<commit_message>
Descreve o que foi feito1
</commit_message>
<xml_diff>
--- a/Diario de TRADE.xlsx
+++ b/Diario de TRADE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anibal Mota\MEOCloud\Trading\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anibal Mota\Documents\Projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D034497-7377-4A2A-8E24-4E7B34C24DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871D4A96-169E-4E6A-B5E5-77626CE18419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="456" windowWidth="18192" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24924" yWindow="204" windowWidth="18192" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agosto" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="109">
   <si>
     <t>Dia</t>
   </si>
@@ -356,13 +356,19 @@
   </si>
   <si>
     <t>Pré abertura; Vela de rejeição; Passou o SL e depois foi como previsto</t>
+  </si>
+  <si>
+    <t>Partiu tudo; Não parei no prejuiso</t>
+  </si>
+  <si>
+    <t>Per entrada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +409,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -480,7 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -504,6 +518,9 @@
     <xf numFmtId="2" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -843,13 +860,13 @@
   <dimension ref="A1:Q300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N64" sqref="N64:N66"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
@@ -859,10 +876,9 @@
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7.88671875" customWidth="1"/>
     <col min="17" max="17" width="58.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -915,7 +931,7 @@
       </c>
       <c r="P1" s="14">
         <f>24.08+(SUM(L2:L300))</f>
-        <v>108.58</v>
+        <v>123.35</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>7</v>
@@ -3952,102 +3968,150 @@
       <c r="P66" s="3"/>
       <c r="Q66" s="1"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="10"/>
-      <c r="M67" s="1">
-        <f t="shared" si="2"/>
-        <v>108.57999999999997</v>
-      </c>
-      <c r="N67" s="3"/>
-      <c r="O67" s="3">
-        <f t="shared" ref="O67:O130" si="8">(M67-24.08)/24.08</f>
-        <v>3.509136212624584</v>
+    <row r="67" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="A67" s="15">
+        <v>23</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="16"/>
+      <c r="M67" s="15">
+        <v>92.53</v>
+      </c>
+      <c r="N67" s="17">
+        <v>-0.2311</v>
+      </c>
+      <c r="O67" s="17">
+        <v>2.8426</v>
       </c>
       <c r="P67" s="3"/>
       <c r="Q67" s="1"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="A68" s="1">
+        <v>24</v>
+      </c>
+      <c r="B68" s="2">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
+      <c r="F68" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
+      <c r="H68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
-      <c r="L68" s="10"/>
+      <c r="L68" s="10">
+        <v>12</v>
+      </c>
       <c r="M68" s="1">
-        <f t="shared" ref="M68:M131" si="9">M67+L68</f>
-        <v>108.57999999999997</v>
-      </c>
-      <c r="N68" s="3"/>
+        <v>104.53</v>
+      </c>
+      <c r="N68" s="3">
+        <v>0.12970000000000001</v>
+      </c>
       <c r="O68" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <v>3.3409</v>
       </c>
       <c r="P68" s="3"/>
-      <c r="Q68" s="1"/>
+      <c r="Q68" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="A69" s="1">
+        <v>24</v>
+      </c>
+      <c r="B69" s="2">
+        <v>0.37222222222222223</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+      <c r="F69" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
+      <c r="H69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
-      <c r="L69" s="10"/>
+      <c r="L69" s="10">
+        <v>-3.01</v>
+      </c>
       <c r="M69" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
-      </c>
-      <c r="N69" s="3"/>
+        <v>101.52</v>
+      </c>
+      <c r="N69" s="3">
+        <v>9.7199999999999995E-2</v>
+      </c>
       <c r="O69" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <v>3.2159</v>
       </c>
       <c r="P69" s="3"/>
       <c r="Q69" s="1"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="A70" s="1">
+        <v>24</v>
+      </c>
+      <c r="B70" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="F70" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
+      <c r="H70" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
-      <c r="L70" s="10"/>
+      <c r="L70" s="10">
+        <v>5.78</v>
+      </c>
       <c r="M70" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
-      </c>
-      <c r="N70" s="3"/>
+        <v>107.3</v>
+      </c>
+      <c r="N70" s="3">
+        <v>0.15959999999999999</v>
+      </c>
       <c r="O70" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <v>3.456</v>
       </c>
       <c r="P70" s="3"/>
       <c r="Q70" s="1"/>
@@ -4066,13 +4130,13 @@
       <c r="K71" s="1"/>
       <c r="L71" s="10"/>
       <c r="M71" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" ref="M68:M131" si="8">M70+L71</f>
+        <v>107.3</v>
       </c>
       <c r="N71" s="3"/>
       <c r="O71" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" ref="O67:O130" si="9">(M71-24.08)/24.08</f>
+        <v>3.455980066445183</v>
       </c>
       <c r="P71" s="3"/>
       <c r="Q71" s="1"/>
@@ -4091,13 +4155,13 @@
       <c r="K72" s="1"/>
       <c r="L72" s="10"/>
       <c r="M72" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N72" s="3"/>
       <c r="O72" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P72" s="3"/>
       <c r="Q72" s="1"/>
@@ -4116,13 +4180,13 @@
       <c r="K73" s="1"/>
       <c r="L73" s="10"/>
       <c r="M73" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N73" s="3"/>
       <c r="O73" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P73" s="3"/>
       <c r="Q73" s="1"/>
@@ -4141,13 +4205,13 @@
       <c r="K74" s="1"/>
       <c r="L74" s="10"/>
       <c r="M74" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N74" s="3"/>
       <c r="O74" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P74" s="3"/>
       <c r="Q74" s="1"/>
@@ -4166,13 +4230,13 @@
       <c r="K75" s="1"/>
       <c r="L75" s="10"/>
       <c r="M75" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N75" s="3"/>
       <c r="O75" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P75" s="3"/>
       <c r="Q75" s="1"/>
@@ -4191,13 +4255,13 @@
       <c r="K76" s="1"/>
       <c r="L76" s="10"/>
       <c r="M76" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N76" s="3"/>
       <c r="O76" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P76" s="3"/>
       <c r="Q76" s="1"/>
@@ -4216,13 +4280,13 @@
       <c r="K77" s="1"/>
       <c r="L77" s="10"/>
       <c r="M77" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N77" s="3"/>
       <c r="O77" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P77" s="3"/>
       <c r="Q77" s="1"/>
@@ -4241,13 +4305,13 @@
       <c r="K78" s="1"/>
       <c r="L78" s="10"/>
       <c r="M78" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N78" s="3"/>
       <c r="O78" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P78" s="3"/>
       <c r="Q78" s="1"/>
@@ -4266,13 +4330,13 @@
       <c r="K79" s="1"/>
       <c r="L79" s="10"/>
       <c r="M79" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N79" s="3"/>
       <c r="O79" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P79" s="3"/>
       <c r="Q79" s="1"/>
@@ -4291,13 +4355,13 @@
       <c r="K80" s="1"/>
       <c r="L80" s="10"/>
       <c r="M80" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N80" s="3"/>
       <c r="O80" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P80" s="3"/>
       <c r="Q80" s="1"/>
@@ -4316,13 +4380,13 @@
       <c r="K81" s="1"/>
       <c r="L81" s="10"/>
       <c r="M81" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N81" s="3"/>
       <c r="O81" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P81" s="3"/>
       <c r="Q81" s="1"/>
@@ -4341,13 +4405,13 @@
       <c r="K82" s="1"/>
       <c r="L82" s="10"/>
       <c r="M82" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N82" s="3"/>
       <c r="O82" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P82" s="3"/>
       <c r="Q82" s="1"/>
@@ -4366,13 +4430,13 @@
       <c r="K83" s="1"/>
       <c r="L83" s="10"/>
       <c r="M83" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N83" s="3"/>
       <c r="O83" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P83" s="3"/>
       <c r="Q83" s="1"/>
@@ -4391,13 +4455,13 @@
       <c r="K84" s="1"/>
       <c r="L84" s="10"/>
       <c r="M84" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N84" s="3"/>
       <c r="O84" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P84" s="3"/>
       <c r="Q84" s="1"/>
@@ -4416,13 +4480,13 @@
       <c r="K85" s="1"/>
       <c r="L85" s="10"/>
       <c r="M85" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N85" s="3"/>
       <c r="O85" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P85" s="3"/>
       <c r="Q85" s="1"/>
@@ -4441,13 +4505,13 @@
       <c r="K86" s="1"/>
       <c r="L86" s="10"/>
       <c r="M86" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N86" s="3"/>
       <c r="O86" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P86" s="3"/>
       <c r="Q86" s="1"/>
@@ -4466,13 +4530,13 @@
       <c r="K87" s="1"/>
       <c r="L87" s="10"/>
       <c r="M87" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N87" s="3"/>
       <c r="O87" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P87" s="3"/>
       <c r="Q87" s="1"/>
@@ -4491,13 +4555,13 @@
       <c r="K88" s="1"/>
       <c r="L88" s="10"/>
       <c r="M88" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N88" s="3"/>
       <c r="O88" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P88" s="3"/>
       <c r="Q88" s="1"/>
@@ -4516,13 +4580,13 @@
       <c r="K89" s="1"/>
       <c r="L89" s="10"/>
       <c r="M89" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N89" s="3"/>
       <c r="O89" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P89" s="3"/>
       <c r="Q89" s="1"/>
@@ -4541,13 +4605,13 @@
       <c r="K90" s="1"/>
       <c r="L90" s="10"/>
       <c r="M90" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N90" s="3"/>
       <c r="O90" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P90" s="3"/>
       <c r="Q90" s="1"/>
@@ -4566,13 +4630,13 @@
       <c r="K91" s="1"/>
       <c r="L91" s="10"/>
       <c r="M91" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N91" s="3"/>
       <c r="O91" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P91" s="3"/>
       <c r="Q91" s="1"/>
@@ -4591,13 +4655,13 @@
       <c r="K92" s="1"/>
       <c r="L92" s="10"/>
       <c r="M92" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N92" s="3"/>
       <c r="O92" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P92" s="3"/>
       <c r="Q92" s="1"/>
@@ -4616,13 +4680,13 @@
       <c r="K93" s="1"/>
       <c r="L93" s="10"/>
       <c r="M93" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N93" s="3"/>
       <c r="O93" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P93" s="3"/>
       <c r="Q93" s="1"/>
@@ -4641,13 +4705,13 @@
       <c r="K94" s="1"/>
       <c r="L94" s="10"/>
       <c r="M94" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N94" s="3"/>
       <c r="O94" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P94" s="3"/>
       <c r="Q94" s="1"/>
@@ -4666,13 +4730,13 @@
       <c r="K95" s="1"/>
       <c r="L95" s="10"/>
       <c r="M95" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N95" s="3"/>
       <c r="O95" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P95" s="3"/>
       <c r="Q95" s="1"/>
@@ -4691,13 +4755,13 @@
       <c r="K96" s="1"/>
       <c r="L96" s="10"/>
       <c r="M96" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N96" s="3"/>
       <c r="O96" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P96" s="3"/>
       <c r="Q96" s="1"/>
@@ -4716,13 +4780,13 @@
       <c r="K97" s="1"/>
       <c r="L97" s="10"/>
       <c r="M97" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N97" s="3"/>
       <c r="O97" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P97" s="3"/>
       <c r="Q97" s="1"/>
@@ -4741,13 +4805,13 @@
       <c r="K98" s="1"/>
       <c r="L98" s="10"/>
       <c r="M98" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N98" s="3"/>
       <c r="O98" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P98" s="3"/>
       <c r="Q98" s="1"/>
@@ -4766,13 +4830,13 @@
       <c r="K99" s="1"/>
       <c r="L99" s="10"/>
       <c r="M99" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N99" s="3"/>
       <c r="O99" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P99" s="3"/>
       <c r="Q99" s="1"/>
@@ -4791,13 +4855,13 @@
       <c r="K100" s="1"/>
       <c r="L100" s="10"/>
       <c r="M100" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N100" s="3"/>
       <c r="O100" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P100" s="3"/>
       <c r="Q100" s="1"/>
@@ -4816,13 +4880,13 @@
       <c r="K101" s="1"/>
       <c r="L101" s="10"/>
       <c r="M101" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N101" s="3"/>
       <c r="O101" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P101" s="3"/>
       <c r="Q101" s="1"/>
@@ -4841,13 +4905,13 @@
       <c r="K102" s="1"/>
       <c r="L102" s="10"/>
       <c r="M102" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N102" s="3"/>
       <c r="O102" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P102" s="3"/>
       <c r="Q102" s="1"/>
@@ -4866,13 +4930,13 @@
       <c r="K103" s="1"/>
       <c r="L103" s="10"/>
       <c r="M103" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N103" s="3"/>
       <c r="O103" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P103" s="3"/>
       <c r="Q103" s="1"/>
@@ -4891,13 +4955,13 @@
       <c r="K104" s="1"/>
       <c r="L104" s="10"/>
       <c r="M104" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N104" s="3"/>
       <c r="O104" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P104" s="3"/>
       <c r="Q104" s="1"/>
@@ -4916,13 +4980,13 @@
       <c r="K105" s="1"/>
       <c r="L105" s="10"/>
       <c r="M105" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N105" s="3"/>
       <c r="O105" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P105" s="3"/>
       <c r="Q105" s="1"/>
@@ -4941,13 +5005,13 @@
       <c r="K106" s="1"/>
       <c r="L106" s="10"/>
       <c r="M106" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N106" s="3"/>
       <c r="O106" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P106" s="3"/>
       <c r="Q106" s="1"/>
@@ -4966,13 +5030,13 @@
       <c r="K107" s="1"/>
       <c r="L107" s="10"/>
       <c r="M107" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N107" s="3"/>
       <c r="O107" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P107" s="3"/>
       <c r="Q107" s="1"/>
@@ -4991,13 +5055,13 @@
       <c r="K108" s="1"/>
       <c r="L108" s="10"/>
       <c r="M108" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N108" s="3"/>
       <c r="O108" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P108" s="3"/>
       <c r="Q108" s="1"/>
@@ -5016,13 +5080,13 @@
       <c r="K109" s="1"/>
       <c r="L109" s="10"/>
       <c r="M109" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N109" s="3"/>
       <c r="O109" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P109" s="3"/>
       <c r="Q109" s="1"/>
@@ -5041,13 +5105,13 @@
       <c r="K110" s="1"/>
       <c r="L110" s="10"/>
       <c r="M110" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N110" s="3"/>
       <c r="O110" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P110" s="3"/>
       <c r="Q110" s="1"/>
@@ -5066,13 +5130,13 @@
       <c r="K111" s="1"/>
       <c r="L111" s="10"/>
       <c r="M111" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N111" s="3"/>
       <c r="O111" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P111" s="3"/>
       <c r="Q111" s="1"/>
@@ -5091,13 +5155,13 @@
       <c r="K112" s="1"/>
       <c r="L112" s="10"/>
       <c r="M112" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N112" s="3"/>
       <c r="O112" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P112" s="3"/>
       <c r="Q112" s="1"/>
@@ -5116,13 +5180,13 @@
       <c r="K113" s="1"/>
       <c r="L113" s="10"/>
       <c r="M113" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N113" s="3"/>
       <c r="O113" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P113" s="3"/>
       <c r="Q113" s="1"/>
@@ -5141,13 +5205,13 @@
       <c r="K114" s="1"/>
       <c r="L114" s="10"/>
       <c r="M114" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N114" s="3"/>
       <c r="O114" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P114" s="3"/>
       <c r="Q114" s="1"/>
@@ -5166,13 +5230,13 @@
       <c r="K115" s="1"/>
       <c r="L115" s="10"/>
       <c r="M115" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N115" s="3"/>
       <c r="O115" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P115" s="3"/>
       <c r="Q115" s="1"/>
@@ -5191,13 +5255,13 @@
       <c r="K116" s="1"/>
       <c r="L116" s="10"/>
       <c r="M116" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N116" s="3"/>
       <c r="O116" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P116" s="3"/>
       <c r="Q116" s="1"/>
@@ -5216,13 +5280,13 @@
       <c r="K117" s="1"/>
       <c r="L117" s="10"/>
       <c r="M117" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N117" s="3"/>
       <c r="O117" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P117" s="3"/>
       <c r="Q117" s="1"/>
@@ -5241,13 +5305,13 @@
       <c r="K118" s="1"/>
       <c r="L118" s="10"/>
       <c r="M118" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N118" s="3"/>
       <c r="O118" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P118" s="3"/>
       <c r="Q118" s="1"/>
@@ -5266,13 +5330,13 @@
       <c r="K119" s="1"/>
       <c r="L119" s="10"/>
       <c r="M119" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N119" s="3"/>
       <c r="O119" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P119" s="3"/>
       <c r="Q119" s="1"/>
@@ -5291,13 +5355,13 @@
       <c r="K120" s="1"/>
       <c r="L120" s="10"/>
       <c r="M120" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N120" s="3"/>
       <c r="O120" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P120" s="3"/>
       <c r="Q120" s="1"/>
@@ -5316,13 +5380,13 @@
       <c r="K121" s="1"/>
       <c r="L121" s="10"/>
       <c r="M121" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N121" s="3"/>
       <c r="O121" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P121" s="3"/>
       <c r="Q121" s="1"/>
@@ -5341,13 +5405,13 @@
       <c r="K122" s="1"/>
       <c r="L122" s="10"/>
       <c r="M122" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N122" s="3"/>
       <c r="O122" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P122" s="3"/>
       <c r="Q122" s="1"/>
@@ -5366,13 +5430,13 @@
       <c r="K123" s="1"/>
       <c r="L123" s="10"/>
       <c r="M123" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N123" s="3"/>
       <c r="O123" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P123" s="3"/>
       <c r="Q123" s="1"/>
@@ -5391,13 +5455,13 @@
       <c r="K124" s="1"/>
       <c r="L124" s="10"/>
       <c r="M124" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N124" s="3"/>
       <c r="O124" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P124" s="3"/>
       <c r="Q124" s="1"/>
@@ -5416,13 +5480,13 @@
       <c r="K125" s="1"/>
       <c r="L125" s="10"/>
       <c r="M125" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N125" s="3"/>
       <c r="O125" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P125" s="3"/>
       <c r="Q125" s="1"/>
@@ -5441,13 +5505,13 @@
       <c r="K126" s="1"/>
       <c r="L126" s="10"/>
       <c r="M126" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N126" s="3"/>
       <c r="O126" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P126" s="3"/>
       <c r="Q126" s="1"/>
@@ -5466,13 +5530,13 @@
       <c r="K127" s="1"/>
       <c r="L127" s="10"/>
       <c r="M127" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N127" s="3"/>
       <c r="O127" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P127" s="3"/>
       <c r="Q127" s="1"/>
@@ -5491,13 +5555,13 @@
       <c r="K128" s="1"/>
       <c r="L128" s="10"/>
       <c r="M128" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N128" s="3"/>
       <c r="O128" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P128" s="3"/>
       <c r="Q128" s="1"/>
@@ -5516,13 +5580,13 @@
       <c r="K129" s="1"/>
       <c r="L129" s="10"/>
       <c r="M129" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N129" s="3"/>
       <c r="O129" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P129" s="3"/>
       <c r="Q129" s="1"/>
@@ -5541,13 +5605,13 @@
       <c r="K130" s="1"/>
       <c r="L130" s="10"/>
       <c r="M130" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N130" s="3"/>
       <c r="O130" s="3">
-        <f t="shared" si="8"/>
-        <v>3.509136212624584</v>
+        <f t="shared" si="9"/>
+        <v>3.455980066445183</v>
       </c>
       <c r="P130" s="3"/>
       <c r="Q130" s="1"/>
@@ -5566,13 +5630,13 @@
       <c r="K131" s="1"/>
       <c r="L131" s="10"/>
       <c r="M131" s="1">
-        <f t="shared" si="9"/>
-        <v>108.57999999999997</v>
+        <f t="shared" si="8"/>
+        <v>107.3</v>
       </c>
       <c r="N131" s="3"/>
       <c r="O131" s="3">
         <f t="shared" ref="O131:O194" si="10">(M131-24.08)/24.08</f>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P131" s="3"/>
       <c r="Q131" s="1"/>
@@ -5592,12 +5656,12 @@
       <c r="L132" s="10"/>
       <c r="M132" s="1">
         <f t="shared" ref="M132:M195" si="11">M131+L132</f>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N132" s="3"/>
       <c r="O132" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P132" s="3"/>
       <c r="Q132" s="1"/>
@@ -5617,12 +5681,12 @@
       <c r="L133" s="10"/>
       <c r="M133" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N133" s="3"/>
       <c r="O133" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P133" s="3"/>
       <c r="Q133" s="1"/>
@@ -5642,12 +5706,12 @@
       <c r="L134" s="10"/>
       <c r="M134" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N134" s="3"/>
       <c r="O134" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P134" s="3"/>
       <c r="Q134" s="1"/>
@@ -5667,12 +5731,12 @@
       <c r="L135" s="10"/>
       <c r="M135" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N135" s="3"/>
       <c r="O135" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P135" s="3"/>
       <c r="Q135" s="1"/>
@@ -5692,12 +5756,12 @@
       <c r="L136" s="10"/>
       <c r="M136" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N136" s="3"/>
       <c r="O136" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P136" s="3"/>
       <c r="Q136" s="1"/>
@@ -5717,12 +5781,12 @@
       <c r="L137" s="10"/>
       <c r="M137" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N137" s="3"/>
       <c r="O137" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P137" s="3"/>
       <c r="Q137" s="1"/>
@@ -5742,12 +5806,12 @@
       <c r="L138" s="10"/>
       <c r="M138" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N138" s="3"/>
       <c r="O138" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P138" s="3"/>
       <c r="Q138" s="1"/>
@@ -5767,12 +5831,12 @@
       <c r="L139" s="10"/>
       <c r="M139" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N139" s="3"/>
       <c r="O139" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P139" s="3"/>
       <c r="Q139" s="1"/>
@@ -5792,12 +5856,12 @@
       <c r="L140" s="10"/>
       <c r="M140" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N140" s="3"/>
       <c r="O140" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P140" s="3"/>
       <c r="Q140" s="1"/>
@@ -5817,12 +5881,12 @@
       <c r="L141" s="10"/>
       <c r="M141" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N141" s="3"/>
       <c r="O141" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P141" s="3"/>
       <c r="Q141" s="1"/>
@@ -5842,12 +5906,12 @@
       <c r="L142" s="10"/>
       <c r="M142" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N142" s="3"/>
       <c r="O142" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P142" s="3"/>
       <c r="Q142" s="1"/>
@@ -5867,12 +5931,12 @@
       <c r="L143" s="10"/>
       <c r="M143" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N143" s="3"/>
       <c r="O143" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P143" s="3"/>
       <c r="Q143" s="1"/>
@@ -5892,12 +5956,12 @@
       <c r="L144" s="10"/>
       <c r="M144" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N144" s="3"/>
       <c r="O144" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P144" s="3"/>
       <c r="Q144" s="1"/>
@@ -5917,12 +5981,12 @@
       <c r="L145" s="10"/>
       <c r="M145" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N145" s="3"/>
       <c r="O145" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P145" s="3"/>
       <c r="Q145" s="1"/>
@@ -5942,12 +6006,12 @@
       <c r="L146" s="10"/>
       <c r="M146" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N146" s="3"/>
       <c r="O146" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P146" s="3"/>
       <c r="Q146" s="1"/>
@@ -5967,12 +6031,12 @@
       <c r="L147" s="10"/>
       <c r="M147" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N147" s="3"/>
       <c r="O147" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P147" s="3"/>
       <c r="Q147" s="1"/>
@@ -5992,12 +6056,12 @@
       <c r="L148" s="10"/>
       <c r="M148" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N148" s="3"/>
       <c r="O148" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P148" s="3"/>
       <c r="Q148" s="1"/>
@@ -6017,12 +6081,12 @@
       <c r="L149" s="10"/>
       <c r="M149" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N149" s="3"/>
       <c r="O149" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P149" s="3"/>
       <c r="Q149" s="1"/>
@@ -6042,12 +6106,12 @@
       <c r="L150" s="10"/>
       <c r="M150" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N150" s="3"/>
       <c r="O150" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P150" s="3"/>
       <c r="Q150" s="1"/>
@@ -6067,12 +6131,12 @@
       <c r="L151" s="10"/>
       <c r="M151" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N151" s="3"/>
       <c r="O151" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P151" s="3"/>
       <c r="Q151" s="1"/>
@@ -6092,12 +6156,12 @@
       <c r="L152" s="10"/>
       <c r="M152" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N152" s="3"/>
       <c r="O152" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P152" s="3"/>
       <c r="Q152" s="1"/>
@@ -6117,12 +6181,12 @@
       <c r="L153" s="10"/>
       <c r="M153" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N153" s="3"/>
       <c r="O153" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P153" s="3"/>
       <c r="Q153" s="1"/>
@@ -6142,12 +6206,12 @@
       <c r="L154" s="10"/>
       <c r="M154" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N154" s="3"/>
       <c r="O154" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P154" s="3"/>
       <c r="Q154" s="1"/>
@@ -6167,12 +6231,12 @@
       <c r="L155" s="10"/>
       <c r="M155" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N155" s="3"/>
       <c r="O155" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P155" s="3"/>
       <c r="Q155" s="1"/>
@@ -6192,12 +6256,12 @@
       <c r="L156" s="10"/>
       <c r="M156" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N156" s="3"/>
       <c r="O156" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P156" s="3"/>
       <c r="Q156" s="1"/>
@@ -6217,12 +6281,12 @@
       <c r="L157" s="10"/>
       <c r="M157" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N157" s="3"/>
       <c r="O157" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P157" s="3"/>
       <c r="Q157" s="1"/>
@@ -6242,12 +6306,12 @@
       <c r="L158" s="10"/>
       <c r="M158" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N158" s="3"/>
       <c r="O158" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P158" s="3"/>
       <c r="Q158" s="1"/>
@@ -6267,12 +6331,12 @@
       <c r="L159" s="10"/>
       <c r="M159" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N159" s="3"/>
       <c r="O159" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P159" s="3"/>
       <c r="Q159" s="1"/>
@@ -6292,12 +6356,12 @@
       <c r="L160" s="10"/>
       <c r="M160" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N160" s="3"/>
       <c r="O160" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P160" s="3"/>
       <c r="Q160" s="1"/>
@@ -6317,12 +6381,12 @@
       <c r="L161" s="10"/>
       <c r="M161" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N161" s="3"/>
       <c r="O161" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P161" s="3"/>
       <c r="Q161" s="1"/>
@@ -6342,12 +6406,12 @@
       <c r="L162" s="10"/>
       <c r="M162" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N162" s="3"/>
       <c r="O162" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P162" s="3"/>
       <c r="Q162" s="1"/>
@@ -6367,12 +6431,12 @@
       <c r="L163" s="10"/>
       <c r="M163" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N163" s="3"/>
       <c r="O163" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P163" s="3"/>
       <c r="Q163" s="1"/>
@@ -6392,12 +6456,12 @@
       <c r="L164" s="10"/>
       <c r="M164" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N164" s="3"/>
       <c r="O164" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P164" s="3"/>
       <c r="Q164" s="1"/>
@@ -6417,12 +6481,12 @@
       <c r="L165" s="10"/>
       <c r="M165" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N165" s="3"/>
       <c r="O165" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P165" s="3"/>
       <c r="Q165" s="1"/>
@@ -6442,12 +6506,12 @@
       <c r="L166" s="10"/>
       <c r="M166" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N166" s="3"/>
       <c r="O166" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P166" s="3"/>
       <c r="Q166" s="1"/>
@@ -6467,12 +6531,12 @@
       <c r="L167" s="10"/>
       <c r="M167" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N167" s="3"/>
       <c r="O167" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P167" s="3"/>
       <c r="Q167" s="1"/>
@@ -6492,12 +6556,12 @@
       <c r="L168" s="10"/>
       <c r="M168" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N168" s="3"/>
       <c r="O168" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P168" s="3"/>
       <c r="Q168" s="1"/>
@@ -6517,12 +6581,12 @@
       <c r="L169" s="10"/>
       <c r="M169" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N169" s="3"/>
       <c r="O169" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P169" s="3"/>
       <c r="Q169" s="1"/>
@@ -6542,12 +6606,12 @@
       <c r="L170" s="10"/>
       <c r="M170" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N170" s="3"/>
       <c r="O170" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P170" s="3"/>
       <c r="Q170" s="1"/>
@@ -6567,12 +6631,12 @@
       <c r="L171" s="10"/>
       <c r="M171" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N171" s="3"/>
       <c r="O171" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P171" s="3"/>
       <c r="Q171" s="1"/>
@@ -6592,12 +6656,12 @@
       <c r="L172" s="10"/>
       <c r="M172" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N172" s="3"/>
       <c r="O172" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P172" s="3"/>
       <c r="Q172" s="1"/>
@@ -6617,12 +6681,12 @@
       <c r="L173" s="10"/>
       <c r="M173" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N173" s="3"/>
       <c r="O173" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P173" s="3"/>
       <c r="Q173" s="1"/>
@@ -6642,12 +6706,12 @@
       <c r="L174" s="10"/>
       <c r="M174" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N174" s="3"/>
       <c r="O174" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P174" s="3"/>
       <c r="Q174" s="1"/>
@@ -6667,12 +6731,12 @@
       <c r="L175" s="10"/>
       <c r="M175" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N175" s="3"/>
       <c r="O175" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P175" s="3"/>
       <c r="Q175" s="1"/>
@@ -6692,12 +6756,12 @@
       <c r="L176" s="10"/>
       <c r="M176" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N176" s="3"/>
       <c r="O176" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P176" s="3"/>
       <c r="Q176" s="1"/>
@@ -6717,12 +6781,12 @@
       <c r="L177" s="10"/>
       <c r="M177" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N177" s="3"/>
       <c r="O177" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P177" s="3"/>
       <c r="Q177" s="1"/>
@@ -6742,12 +6806,12 @@
       <c r="L178" s="10"/>
       <c r="M178" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N178" s="3"/>
       <c r="O178" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P178" s="3"/>
       <c r="Q178" s="1"/>
@@ -6767,12 +6831,12 @@
       <c r="L179" s="10"/>
       <c r="M179" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N179" s="3"/>
       <c r="O179" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P179" s="3"/>
       <c r="Q179" s="1"/>
@@ -6792,12 +6856,12 @@
       <c r="L180" s="10"/>
       <c r="M180" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N180" s="3"/>
       <c r="O180" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P180" s="3"/>
       <c r="Q180" s="1"/>
@@ -6817,12 +6881,12 @@
       <c r="L181" s="10"/>
       <c r="M181" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N181" s="3"/>
       <c r="O181" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P181" s="3"/>
       <c r="Q181" s="1"/>
@@ -6842,12 +6906,12 @@
       <c r="L182" s="10"/>
       <c r="M182" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N182" s="3"/>
       <c r="O182" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P182" s="3"/>
       <c r="Q182" s="1"/>
@@ -6867,12 +6931,12 @@
       <c r="L183" s="10"/>
       <c r="M183" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N183" s="3"/>
       <c r="O183" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P183" s="3"/>
       <c r="Q183" s="1"/>
@@ -6892,12 +6956,12 @@
       <c r="L184" s="10"/>
       <c r="M184" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N184" s="3"/>
       <c r="O184" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P184" s="3"/>
       <c r="Q184" s="1"/>
@@ -6917,12 +6981,12 @@
       <c r="L185" s="10"/>
       <c r="M185" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N185" s="3"/>
       <c r="O185" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P185" s="3"/>
       <c r="Q185" s="1"/>
@@ -6942,12 +7006,12 @@
       <c r="L186" s="10"/>
       <c r="M186" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N186" s="3"/>
       <c r="O186" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P186" s="3"/>
       <c r="Q186" s="1"/>
@@ -6967,12 +7031,12 @@
       <c r="L187" s="10"/>
       <c r="M187" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N187" s="3"/>
       <c r="O187" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P187" s="3"/>
       <c r="Q187" s="1"/>
@@ -6992,12 +7056,12 @@
       <c r="L188" s="10"/>
       <c r="M188" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N188" s="3"/>
       <c r="O188" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P188" s="3"/>
       <c r="Q188" s="1"/>
@@ -7017,12 +7081,12 @@
       <c r="L189" s="10"/>
       <c r="M189" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N189" s="3"/>
       <c r="O189" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P189" s="3"/>
       <c r="Q189" s="1"/>
@@ -7042,12 +7106,12 @@
       <c r="L190" s="10"/>
       <c r="M190" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N190" s="3"/>
       <c r="O190" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P190" s="3"/>
       <c r="Q190" s="1"/>
@@ -7067,12 +7131,12 @@
       <c r="L191" s="10"/>
       <c r="M191" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N191" s="3"/>
       <c r="O191" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P191" s="3"/>
       <c r="Q191" s="1"/>
@@ -7092,12 +7156,12 @@
       <c r="L192" s="10"/>
       <c r="M192" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N192" s="3"/>
       <c r="O192" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P192" s="3"/>
       <c r="Q192" s="1"/>
@@ -7117,12 +7181,12 @@
       <c r="L193" s="10"/>
       <c r="M193" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N193" s="3"/>
       <c r="O193" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P193" s="3"/>
       <c r="Q193" s="1"/>
@@ -7142,12 +7206,12 @@
       <c r="L194" s="10"/>
       <c r="M194" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N194" s="3"/>
       <c r="O194" s="3">
         <f t="shared" si="10"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P194" s="3"/>
       <c r="Q194" s="1"/>
@@ -7167,12 +7231,12 @@
       <c r="L195" s="10"/>
       <c r="M195" s="1">
         <f t="shared" si="11"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N195" s="3"/>
       <c r="O195" s="3">
         <f t="shared" ref="O195:O258" si="12">(M195-24.08)/24.08</f>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P195" s="3"/>
       <c r="Q195" s="1"/>
@@ -7192,12 +7256,12 @@
       <c r="L196" s="10"/>
       <c r="M196" s="1">
         <f t="shared" ref="M196:M259" si="13">M195+L196</f>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N196" s="3"/>
       <c r="O196" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P196" s="3"/>
       <c r="Q196" s="1"/>
@@ -7217,12 +7281,12 @@
       <c r="L197" s="10"/>
       <c r="M197" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N197" s="3"/>
       <c r="O197" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P197" s="3"/>
       <c r="Q197" s="1"/>
@@ -7242,12 +7306,12 @@
       <c r="L198" s="10"/>
       <c r="M198" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N198" s="3"/>
       <c r="O198" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P198" s="3"/>
       <c r="Q198" s="1"/>
@@ -7267,12 +7331,12 @@
       <c r="L199" s="10"/>
       <c r="M199" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N199" s="3"/>
       <c r="O199" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P199" s="3"/>
       <c r="Q199" s="1"/>
@@ -7292,12 +7356,12 @@
       <c r="L200" s="10"/>
       <c r="M200" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N200" s="3"/>
       <c r="O200" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P200" s="3"/>
       <c r="Q200" s="1"/>
@@ -7317,12 +7381,12 @@
       <c r="L201" s="10"/>
       <c r="M201" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N201" s="3"/>
       <c r="O201" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P201" s="3"/>
       <c r="Q201" s="1"/>
@@ -7342,12 +7406,12 @@
       <c r="L202" s="10"/>
       <c r="M202" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N202" s="3"/>
       <c r="O202" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P202" s="3"/>
       <c r="Q202" s="1"/>
@@ -7367,12 +7431,12 @@
       <c r="L203" s="10"/>
       <c r="M203" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N203" s="3"/>
       <c r="O203" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P203" s="3"/>
       <c r="Q203" s="1"/>
@@ -7392,12 +7456,12 @@
       <c r="L204" s="10"/>
       <c r="M204" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N204" s="3"/>
       <c r="O204" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P204" s="3"/>
       <c r="Q204" s="1"/>
@@ -7417,12 +7481,12 @@
       <c r="L205" s="10"/>
       <c r="M205" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N205" s="3"/>
       <c r="O205" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P205" s="3"/>
       <c r="Q205" s="1"/>
@@ -7442,12 +7506,12 @@
       <c r="L206" s="10"/>
       <c r="M206" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N206" s="3"/>
       <c r="O206" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P206" s="3"/>
       <c r="Q206" s="1"/>
@@ -7467,12 +7531,12 @@
       <c r="L207" s="10"/>
       <c r="M207" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N207" s="3"/>
       <c r="O207" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P207" s="3"/>
       <c r="Q207" s="1"/>
@@ -7492,12 +7556,12 @@
       <c r="L208" s="10"/>
       <c r="M208" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N208" s="3"/>
       <c r="O208" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P208" s="3"/>
       <c r="Q208" s="1"/>
@@ -7517,12 +7581,12 @@
       <c r="L209" s="10"/>
       <c r="M209" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N209" s="3"/>
       <c r="O209" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P209" s="3"/>
       <c r="Q209" s="1"/>
@@ -7542,12 +7606,12 @@
       <c r="L210" s="10"/>
       <c r="M210" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N210" s="3"/>
       <c r="O210" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P210" s="3"/>
       <c r="Q210" s="1"/>
@@ -7567,12 +7631,12 @@
       <c r="L211" s="10"/>
       <c r="M211" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N211" s="3"/>
       <c r="O211" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P211" s="3"/>
       <c r="Q211" s="1"/>
@@ -7592,12 +7656,12 @@
       <c r="L212" s="10"/>
       <c r="M212" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N212" s="3"/>
       <c r="O212" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P212" s="3"/>
       <c r="Q212" s="1"/>
@@ -7617,12 +7681,12 @@
       <c r="L213" s="10"/>
       <c r="M213" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N213" s="3"/>
       <c r="O213" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P213" s="3"/>
       <c r="Q213" s="1"/>
@@ -7642,12 +7706,12 @@
       <c r="L214" s="10"/>
       <c r="M214" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N214" s="3"/>
       <c r="O214" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P214" s="3"/>
       <c r="Q214" s="1"/>
@@ -7667,12 +7731,12 @@
       <c r="L215" s="10"/>
       <c r="M215" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N215" s="3"/>
       <c r="O215" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P215" s="3"/>
       <c r="Q215" s="1"/>
@@ -7692,12 +7756,12 @@
       <c r="L216" s="10"/>
       <c r="M216" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N216" s="3"/>
       <c r="O216" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P216" s="3"/>
       <c r="Q216" s="1"/>
@@ -7717,12 +7781,12 @@
       <c r="L217" s="10"/>
       <c r="M217" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N217" s="3"/>
       <c r="O217" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P217" s="3"/>
       <c r="Q217" s="1"/>
@@ -7742,12 +7806,12 @@
       <c r="L218" s="10"/>
       <c r="M218" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N218" s="3"/>
       <c r="O218" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P218" s="3"/>
       <c r="Q218" s="1"/>
@@ -7767,12 +7831,12 @@
       <c r="L219" s="10"/>
       <c r="M219" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N219" s="3"/>
       <c r="O219" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P219" s="3"/>
       <c r="Q219" s="1"/>
@@ -7792,12 +7856,12 @@
       <c r="L220" s="10"/>
       <c r="M220" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N220" s="3"/>
       <c r="O220" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P220" s="3"/>
       <c r="Q220" s="1"/>
@@ -7817,12 +7881,12 @@
       <c r="L221" s="10"/>
       <c r="M221" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N221" s="3"/>
       <c r="O221" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P221" s="3"/>
       <c r="Q221" s="1"/>
@@ -7842,12 +7906,12 @@
       <c r="L222" s="10"/>
       <c r="M222" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N222" s="3"/>
       <c r="O222" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P222" s="3"/>
       <c r="Q222" s="1"/>
@@ -7867,12 +7931,12 @@
       <c r="L223" s="10"/>
       <c r="M223" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N223" s="3"/>
       <c r="O223" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P223" s="3"/>
       <c r="Q223" s="1"/>
@@ -7892,12 +7956,12 @@
       <c r="L224" s="10"/>
       <c r="M224" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N224" s="3"/>
       <c r="O224" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P224" s="3"/>
       <c r="Q224" s="1"/>
@@ -7917,12 +7981,12 @@
       <c r="L225" s="10"/>
       <c r="M225" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N225" s="3"/>
       <c r="O225" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P225" s="3"/>
       <c r="Q225" s="1"/>
@@ -7942,12 +8006,12 @@
       <c r="L226" s="10"/>
       <c r="M226" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N226" s="3"/>
       <c r="O226" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P226" s="3"/>
       <c r="Q226" s="1"/>
@@ -7967,12 +8031,12 @@
       <c r="L227" s="10"/>
       <c r="M227" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N227" s="3"/>
       <c r="O227" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P227" s="3"/>
       <c r="Q227" s="1"/>
@@ -7992,12 +8056,12 @@
       <c r="L228" s="10"/>
       <c r="M228" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N228" s="3"/>
       <c r="O228" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P228" s="3"/>
       <c r="Q228" s="1"/>
@@ -8017,12 +8081,12 @@
       <c r="L229" s="10"/>
       <c r="M229" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N229" s="3"/>
       <c r="O229" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P229" s="3"/>
       <c r="Q229" s="1"/>
@@ -8042,12 +8106,12 @@
       <c r="L230" s="10"/>
       <c r="M230" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N230" s="3"/>
       <c r="O230" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P230" s="3"/>
       <c r="Q230" s="1"/>
@@ -8067,12 +8131,12 @@
       <c r="L231" s="10"/>
       <c r="M231" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N231" s="3"/>
       <c r="O231" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P231" s="3"/>
       <c r="Q231" s="1"/>
@@ -8092,12 +8156,12 @@
       <c r="L232" s="10"/>
       <c r="M232" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N232" s="3"/>
       <c r="O232" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P232" s="3"/>
       <c r="Q232" s="1"/>
@@ -8117,12 +8181,12 @@
       <c r="L233" s="10"/>
       <c r="M233" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N233" s="3"/>
       <c r="O233" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P233" s="3"/>
       <c r="Q233" s="1"/>
@@ -8142,12 +8206,12 @@
       <c r="L234" s="10"/>
       <c r="M234" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N234" s="3"/>
       <c r="O234" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P234" s="3"/>
       <c r="Q234" s="1"/>
@@ -8167,12 +8231,12 @@
       <c r="L235" s="10"/>
       <c r="M235" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N235" s="3"/>
       <c r="O235" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P235" s="3"/>
       <c r="Q235" s="1"/>
@@ -8192,12 +8256,12 @@
       <c r="L236" s="10"/>
       <c r="M236" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N236" s="3"/>
       <c r="O236" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P236" s="3"/>
       <c r="Q236" s="1"/>
@@ -8217,12 +8281,12 @@
       <c r="L237" s="10"/>
       <c r="M237" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N237" s="3"/>
       <c r="O237" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P237" s="3"/>
       <c r="Q237" s="1"/>
@@ -8242,12 +8306,12 @@
       <c r="L238" s="10"/>
       <c r="M238" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N238" s="3"/>
       <c r="O238" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P238" s="3"/>
       <c r="Q238" s="1"/>
@@ -8267,12 +8331,12 @@
       <c r="L239" s="10"/>
       <c r="M239" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N239" s="3"/>
       <c r="O239" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P239" s="3"/>
       <c r="Q239" s="1"/>
@@ -8292,12 +8356,12 @@
       <c r="L240" s="10"/>
       <c r="M240" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N240" s="3"/>
       <c r="O240" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P240" s="3"/>
       <c r="Q240" s="1"/>
@@ -8317,12 +8381,12 @@
       <c r="L241" s="10"/>
       <c r="M241" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N241" s="3"/>
       <c r="O241" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P241" s="3"/>
       <c r="Q241" s="1"/>
@@ -8342,12 +8406,12 @@
       <c r="L242" s="10"/>
       <c r="M242" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N242" s="3"/>
       <c r="O242" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P242" s="3"/>
       <c r="Q242" s="1"/>
@@ -8367,12 +8431,12 @@
       <c r="L243" s="10"/>
       <c r="M243" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N243" s="3"/>
       <c r="O243" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P243" s="3"/>
       <c r="Q243" s="1"/>
@@ -8392,12 +8456,12 @@
       <c r="L244" s="10"/>
       <c r="M244" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N244" s="3"/>
       <c r="O244" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P244" s="3"/>
       <c r="Q244" s="1"/>
@@ -8417,12 +8481,12 @@
       <c r="L245" s="10"/>
       <c r="M245" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N245" s="3"/>
       <c r="O245" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P245" s="3"/>
       <c r="Q245" s="1"/>
@@ -8442,12 +8506,12 @@
       <c r="L246" s="10"/>
       <c r="M246" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N246" s="3"/>
       <c r="O246" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P246" s="3"/>
       <c r="Q246" s="1"/>
@@ -8467,12 +8531,12 @@
       <c r="L247" s="10"/>
       <c r="M247" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N247" s="3"/>
       <c r="O247" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P247" s="3"/>
       <c r="Q247" s="1"/>
@@ -8492,12 +8556,12 @@
       <c r="L248" s="10"/>
       <c r="M248" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N248" s="3"/>
       <c r="O248" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P248" s="3"/>
       <c r="Q248" s="1"/>
@@ -8517,12 +8581,12 @@
       <c r="L249" s="10"/>
       <c r="M249" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N249" s="3"/>
       <c r="O249" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P249" s="3"/>
       <c r="Q249" s="1"/>
@@ -8542,12 +8606,12 @@
       <c r="L250" s="10"/>
       <c r="M250" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N250" s="3"/>
       <c r="O250" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P250" s="3"/>
       <c r="Q250" s="1"/>
@@ -8567,12 +8631,12 @@
       <c r="L251" s="10"/>
       <c r="M251" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N251" s="3"/>
       <c r="O251" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P251" s="3"/>
       <c r="Q251" s="1"/>
@@ -8592,12 +8656,12 @@
       <c r="L252" s="10"/>
       <c r="M252" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N252" s="3"/>
       <c r="O252" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P252" s="3"/>
       <c r="Q252" s="1"/>
@@ -8617,12 +8681,12 @@
       <c r="L253" s="10"/>
       <c r="M253" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N253" s="3"/>
       <c r="O253" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P253" s="3"/>
       <c r="Q253" s="1"/>
@@ -8642,12 +8706,12 @@
       <c r="L254" s="10"/>
       <c r="M254" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N254" s="3"/>
       <c r="O254" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P254" s="3"/>
       <c r="Q254" s="1"/>
@@ -8667,12 +8731,12 @@
       <c r="L255" s="10"/>
       <c r="M255" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N255" s="3"/>
       <c r="O255" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P255" s="3"/>
       <c r="Q255" s="1"/>
@@ -8692,12 +8756,12 @@
       <c r="L256" s="10"/>
       <c r="M256" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N256" s="3"/>
       <c r="O256" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P256" s="3"/>
       <c r="Q256" s="1"/>
@@ -8717,12 +8781,12 @@
       <c r="L257" s="10"/>
       <c r="M257" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N257" s="3"/>
       <c r="O257" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P257" s="3"/>
       <c r="Q257" s="1"/>
@@ -8742,12 +8806,12 @@
       <c r="L258" s="10"/>
       <c r="M258" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N258" s="3"/>
       <c r="O258" s="3">
         <f t="shared" si="12"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P258" s="3"/>
       <c r="Q258" s="1"/>
@@ -8767,12 +8831,12 @@
       <c r="L259" s="10"/>
       <c r="M259" s="1">
         <f t="shared" si="13"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N259" s="3"/>
       <c r="O259" s="3">
         <f t="shared" ref="O259:O300" si="14">(M259-24.08)/24.08</f>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P259" s="3"/>
       <c r="Q259" s="1"/>
@@ -8792,12 +8856,12 @@
       <c r="L260" s="10"/>
       <c r="M260" s="1">
         <f t="shared" ref="M260:M300" si="15">M259+L260</f>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N260" s="3"/>
       <c r="O260" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P260" s="3"/>
       <c r="Q260" s="1"/>
@@ -8817,12 +8881,12 @@
       <c r="L261" s="10"/>
       <c r="M261" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N261" s="3"/>
       <c r="O261" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P261" s="3"/>
       <c r="Q261" s="1"/>
@@ -8842,12 +8906,12 @@
       <c r="L262" s="10"/>
       <c r="M262" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N262" s="3"/>
       <c r="O262" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P262" s="3"/>
       <c r="Q262" s="1"/>
@@ -8867,12 +8931,12 @@
       <c r="L263" s="10"/>
       <c r="M263" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N263" s="3"/>
       <c r="O263" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P263" s="3"/>
       <c r="Q263" s="1"/>
@@ -8892,12 +8956,12 @@
       <c r="L264" s="10"/>
       <c r="M264" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N264" s="3"/>
       <c r="O264" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P264" s="3"/>
       <c r="Q264" s="1"/>
@@ -8917,12 +8981,12 @@
       <c r="L265" s="10"/>
       <c r="M265" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N265" s="3"/>
       <c r="O265" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P265" s="3"/>
       <c r="Q265" s="1"/>
@@ -8942,12 +9006,12 @@
       <c r="L266" s="10"/>
       <c r="M266" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N266" s="3"/>
       <c r="O266" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P266" s="3"/>
       <c r="Q266" s="1"/>
@@ -8967,12 +9031,12 @@
       <c r="L267" s="10"/>
       <c r="M267" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N267" s="3"/>
       <c r="O267" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P267" s="3"/>
       <c r="Q267" s="1"/>
@@ -8992,12 +9056,12 @@
       <c r="L268" s="10"/>
       <c r="M268" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N268" s="3"/>
       <c r="O268" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P268" s="3"/>
       <c r="Q268" s="1"/>
@@ -9017,12 +9081,12 @@
       <c r="L269" s="10"/>
       <c r="M269" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N269" s="3"/>
       <c r="O269" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P269" s="3"/>
       <c r="Q269" s="1"/>
@@ -9042,12 +9106,12 @@
       <c r="L270" s="10"/>
       <c r="M270" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N270" s="3"/>
       <c r="O270" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P270" s="3"/>
       <c r="Q270" s="1"/>
@@ -9067,12 +9131,12 @@
       <c r="L271" s="10"/>
       <c r="M271" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N271" s="3"/>
       <c r="O271" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P271" s="3"/>
       <c r="Q271" s="1"/>
@@ -9092,12 +9156,12 @@
       <c r="L272" s="10"/>
       <c r="M272" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N272" s="3"/>
       <c r="O272" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P272" s="3"/>
       <c r="Q272" s="1"/>
@@ -9117,12 +9181,12 @@
       <c r="L273" s="10"/>
       <c r="M273" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N273" s="3"/>
       <c r="O273" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P273" s="3"/>
       <c r="Q273" s="1"/>
@@ -9142,12 +9206,12 @@
       <c r="L274" s="10"/>
       <c r="M274" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N274" s="3"/>
       <c r="O274" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P274" s="3"/>
       <c r="Q274" s="1"/>
@@ -9167,12 +9231,12 @@
       <c r="L275" s="10"/>
       <c r="M275" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N275" s="3"/>
       <c r="O275" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P275" s="3"/>
       <c r="Q275" s="1"/>
@@ -9192,12 +9256,12 @@
       <c r="L276" s="10"/>
       <c r="M276" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N276" s="3"/>
       <c r="O276" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P276" s="3"/>
       <c r="Q276" s="1"/>
@@ -9217,12 +9281,12 @@
       <c r="L277" s="10"/>
       <c r="M277" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N277" s="3"/>
       <c r="O277" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P277" s="3"/>
       <c r="Q277" s="1"/>
@@ -9242,12 +9306,12 @@
       <c r="L278" s="10"/>
       <c r="M278" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N278" s="3"/>
       <c r="O278" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P278" s="3"/>
       <c r="Q278" s="1"/>
@@ -9267,12 +9331,12 @@
       <c r="L279" s="10"/>
       <c r="M279" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N279" s="3"/>
       <c r="O279" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P279" s="3"/>
       <c r="Q279" s="1"/>
@@ -9292,12 +9356,12 @@
       <c r="L280" s="10"/>
       <c r="M280" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N280" s="3"/>
       <c r="O280" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P280" s="3"/>
       <c r="Q280" s="1"/>
@@ -9317,12 +9381,12 @@
       <c r="L281" s="10"/>
       <c r="M281" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N281" s="3"/>
       <c r="O281" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P281" s="3"/>
       <c r="Q281" s="1"/>
@@ -9342,12 +9406,12 @@
       <c r="L282" s="10"/>
       <c r="M282" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N282" s="3"/>
       <c r="O282" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P282" s="3"/>
       <c r="Q282" s="1"/>
@@ -9367,12 +9431,12 @@
       <c r="L283" s="10"/>
       <c r="M283" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N283" s="3"/>
       <c r="O283" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P283" s="3"/>
       <c r="Q283" s="1"/>
@@ -9392,12 +9456,12 @@
       <c r="L284" s="10"/>
       <c r="M284" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N284" s="3"/>
       <c r="O284" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P284" s="3"/>
       <c r="Q284" s="1"/>
@@ -9417,12 +9481,12 @@
       <c r="L285" s="10"/>
       <c r="M285" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N285" s="3"/>
       <c r="O285" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P285" s="3"/>
       <c r="Q285" s="1"/>
@@ -9442,12 +9506,12 @@
       <c r="L286" s="10"/>
       <c r="M286" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N286" s="3"/>
       <c r="O286" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P286" s="3"/>
       <c r="Q286" s="1"/>
@@ -9467,12 +9531,12 @@
       <c r="L287" s="10"/>
       <c r="M287" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N287" s="3"/>
       <c r="O287" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P287" s="3"/>
       <c r="Q287" s="1"/>
@@ -9492,12 +9556,12 @@
       <c r="L288" s="10"/>
       <c r="M288" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N288" s="3"/>
       <c r="O288" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P288" s="3"/>
       <c r="Q288" s="1"/>
@@ -9517,12 +9581,12 @@
       <c r="L289" s="10"/>
       <c r="M289" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N289" s="3"/>
       <c r="O289" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P289" s="3"/>
       <c r="Q289" s="1"/>
@@ -9542,12 +9606,12 @@
       <c r="L290" s="10"/>
       <c r="M290" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N290" s="3"/>
       <c r="O290" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P290" s="3"/>
       <c r="Q290" s="1"/>
@@ -9567,12 +9631,12 @@
       <c r="L291" s="10"/>
       <c r="M291" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N291" s="3"/>
       <c r="O291" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P291" s="3"/>
       <c r="Q291" s="1"/>
@@ -9592,12 +9656,12 @@
       <c r="L292" s="10"/>
       <c r="M292" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N292" s="3"/>
       <c r="O292" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P292" s="3"/>
       <c r="Q292" s="1"/>
@@ -9617,12 +9681,12 @@
       <c r="L293" s="10"/>
       <c r="M293" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N293" s="3"/>
       <c r="O293" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P293" s="3"/>
       <c r="Q293" s="1"/>
@@ -9642,12 +9706,12 @@
       <c r="L294" s="10"/>
       <c r="M294" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N294" s="3"/>
       <c r="O294" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P294" s="3"/>
       <c r="Q294" s="1"/>
@@ -9667,12 +9731,12 @@
       <c r="L295" s="10"/>
       <c r="M295" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N295" s="3"/>
       <c r="O295" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P295" s="3"/>
       <c r="Q295" s="1"/>
@@ -9692,12 +9756,12 @@
       <c r="L296" s="10"/>
       <c r="M296" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N296" s="3"/>
       <c r="O296" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P296" s="3"/>
       <c r="Q296" s="1"/>
@@ -9717,12 +9781,12 @@
       <c r="L297" s="10"/>
       <c r="M297" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N297" s="3"/>
       <c r="O297" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P297" s="3"/>
       <c r="Q297" s="1"/>
@@ -9742,12 +9806,12 @@
       <c r="L298" s="10"/>
       <c r="M298" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N298" s="3"/>
       <c r="O298" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P298" s="3"/>
       <c r="Q298" s="1"/>
@@ -9767,12 +9831,12 @@
       <c r="L299" s="10"/>
       <c r="M299" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N299" s="3"/>
       <c r="O299" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P299" s="3"/>
       <c r="Q299" s="1"/>
@@ -9792,12 +9856,12 @@
       <c r="L300" s="10"/>
       <c r="M300" s="1">
         <f t="shared" si="15"/>
-        <v>108.57999999999997</v>
+        <v>107.3</v>
       </c>
       <c r="N300" s="3"/>
       <c r="O300" s="3">
         <f t="shared" si="14"/>
-        <v>3.509136212624584</v>
+        <v>3.455980066445183</v>
       </c>
       <c r="P300" s="3"/>
       <c r="Q300" s="1"/>

</xml_diff>

<commit_message>
Foi inserido novo ficheiro Calculadora e foi atualizado o diario de trade
</commit_message>
<xml_diff>
--- a/Diario de TRADE.xlsx
+++ b/Diario de TRADE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anibal Mota\Documents\Projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5A0965-44F2-4E29-8454-175F9FBFC1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652F4777-C299-4F67-BBE1-397C6E3DC6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24924" yWindow="204" windowWidth="18192" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agosto" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="110">
   <si>
     <t>Dia</t>
   </si>
@@ -362,6 +362,9 @@
   </si>
   <si>
     <t>Per entrada</t>
+  </si>
+  <si>
+    <t>ERRO NOVAMENTE EXESSO DE OPERAÇÕES</t>
   </si>
 </sst>
 </file>
@@ -860,8 +863,8 @@
   <dimension ref="A1:Q300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G76" sqref="G76"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74:O74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,7 +935,7 @@
       </c>
       <c r="P1" s="14">
         <f>92.53+SUM(L68:L300)</f>
-        <v>107.3</v>
+        <v>95.97</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>7</v>
@@ -4029,7 +4032,8 @@
         <v>104.53</v>
       </c>
       <c r="N68" s="3">
-        <v>0.12970000000000001</v>
+        <f>(M68-$M$67)/$M$67</f>
+        <v>0.12968766886415217</v>
       </c>
       <c r="O68" s="3">
         <v>3.3409</v>
@@ -4070,7 +4074,8 @@
         <v>101.52</v>
       </c>
       <c r="N69" s="3">
-        <v>9.7199999999999995E-2</v>
+        <f t="shared" ref="N69:N74" si="8">(M69-$M$67)/$M$67</f>
+        <v>9.715767859072727E-2</v>
       </c>
       <c r="O69" s="3">
         <v>3.2159</v>
@@ -4109,7 +4114,8 @@
         <v>107.3</v>
       </c>
       <c r="N70" s="3">
-        <v>0.15959999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.15962390576029392</v>
       </c>
       <c r="O70" s="3">
         <v>3.456</v>
@@ -4118,8 +4124,10 @@
       <c r="Q70" s="1"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
+      <c r="A71" s="1">
+        <v>25</v>
+      </c>
+      <c r="B71" s="2"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -4129,15 +4137,20 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
-      <c r="L71" s="10"/>
+      <c r="L71" s="10">
+        <v>-3.4</v>
+      </c>
       <c r="M71" s="10">
-        <f t="shared" ref="M71:M131" si="8">M70+L71</f>
-        <v>107.3</v>
-      </c>
-      <c r="N71" s="3"/>
+        <f t="shared" ref="M71:M131" si="9">M70+L71</f>
+        <v>103.89999999999999</v>
+      </c>
+      <c r="N71" s="3">
+        <f>(M71-$M$70)/$M$70</f>
+        <v>-3.168685927306622E-2</v>
+      </c>
       <c r="O71" s="3">
-        <f t="shared" ref="O71:O130" si="9">(M71-24.08)/24.08</f>
-        <v>3.455980066445183</v>
+        <f t="shared" ref="O71:O130" si="10">(M71-24.08)/24.08</f>
+        <v>3.3147840531561461</v>
       </c>
       <c r="P71" s="3"/>
       <c r="Q71" s="1"/>
@@ -4154,15 +4167,20 @@
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
-      <c r="L72" s="10"/>
+      <c r="L72" s="10">
+        <v>-7.2</v>
+      </c>
       <c r="M72" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
-      </c>
-      <c r="N72" s="3"/>
+        <f t="shared" si="9"/>
+        <v>96.699999999999989</v>
+      </c>
+      <c r="N72" s="3">
+        <f t="shared" ref="N72:N75" si="11">(M72-$M$70)/$M$70</f>
+        <v>-9.8788443616029911E-2</v>
+      </c>
       <c r="O72" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>3.0157807308970099</v>
       </c>
       <c r="P72" s="3"/>
       <c r="Q72" s="1"/>
@@ -4179,40 +4197,52 @@
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
-      <c r="L73" s="10"/>
+      <c r="L73" s="10">
+        <v>-0.73</v>
+      </c>
       <c r="M73" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
-      </c>
-      <c r="N73" s="3"/>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
+      </c>
+      <c r="N73" s="3">
+        <f t="shared" si="11"/>
+        <v>-0.1055917986952471</v>
+      </c>
       <c r="O73" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P73" s="3"/>
       <c r="Q73" s="1"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="10"/>
-      <c r="M74" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
-      </c>
-      <c r="N74" s="3"/>
-      <c r="O74" s="3">
+    <row r="74" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+      <c r="A74" s="15">
+        <v>25</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="16"/>
+      <c r="M74" s="16">
         <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <v>95.969999999999985</v>
+      </c>
+      <c r="N74" s="17">
+        <f t="shared" si="11"/>
+        <v>-0.1055917986952471</v>
+      </c>
+      <c r="O74" s="17">
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P74" s="3"/>
       <c r="Q74" s="1"/>
@@ -4231,13 +4261,16 @@
       <c r="K75" s="1"/>
       <c r="L75" s="10"/>
       <c r="M75" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
-      </c>
-      <c r="N75" s="3"/>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
+      </c>
+      <c r="N75" s="3">
+        <f>(M75-$M$74)/$M$74</f>
+        <v>0</v>
+      </c>
       <c r="O75" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P75" s="3"/>
       <c r="Q75" s="1"/>
@@ -4256,13 +4289,13 @@
       <c r="K76" s="1"/>
       <c r="L76" s="10"/>
       <c r="M76" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N76" s="3"/>
       <c r="O76" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P76" s="3"/>
       <c r="Q76" s="1"/>
@@ -4281,13 +4314,13 @@
       <c r="K77" s="1"/>
       <c r="L77" s="10"/>
       <c r="M77" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N77" s="3"/>
       <c r="O77" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P77" s="3"/>
       <c r="Q77" s="1"/>
@@ -4306,13 +4339,13 @@
       <c r="K78" s="1"/>
       <c r="L78" s="10"/>
       <c r="M78" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N78" s="3"/>
       <c r="O78" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P78" s="3"/>
       <c r="Q78" s="1"/>
@@ -4331,13 +4364,13 @@
       <c r="K79" s="1"/>
       <c r="L79" s="10"/>
       <c r="M79" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N79" s="3"/>
       <c r="O79" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P79" s="3"/>
       <c r="Q79" s="1"/>
@@ -4356,13 +4389,13 @@
       <c r="K80" s="1"/>
       <c r="L80" s="10"/>
       <c r="M80" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N80" s="3"/>
       <c r="O80" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P80" s="3"/>
       <c r="Q80" s="1"/>
@@ -4381,13 +4414,13 @@
       <c r="K81" s="1"/>
       <c r="L81" s="10"/>
       <c r="M81" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N81" s="3"/>
       <c r="O81" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P81" s="3"/>
       <c r="Q81" s="1"/>
@@ -4406,13 +4439,13 @@
       <c r="K82" s="1"/>
       <c r="L82" s="10"/>
       <c r="M82" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N82" s="3"/>
       <c r="O82" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P82" s="3"/>
       <c r="Q82" s="1"/>
@@ -4431,13 +4464,13 @@
       <c r="K83" s="1"/>
       <c r="L83" s="10"/>
       <c r="M83" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N83" s="3"/>
       <c r="O83" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P83" s="3"/>
       <c r="Q83" s="1"/>
@@ -4456,13 +4489,13 @@
       <c r="K84" s="1"/>
       <c r="L84" s="10"/>
       <c r="M84" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N84" s="3"/>
       <c r="O84" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P84" s="3"/>
       <c r="Q84" s="1"/>
@@ -4481,13 +4514,13 @@
       <c r="K85" s="1"/>
       <c r="L85" s="10"/>
       <c r="M85" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N85" s="3"/>
       <c r="O85" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P85" s="3"/>
       <c r="Q85" s="1"/>
@@ -4506,13 +4539,13 @@
       <c r="K86" s="1"/>
       <c r="L86" s="10"/>
       <c r="M86" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N86" s="3"/>
       <c r="O86" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P86" s="3"/>
       <c r="Q86" s="1"/>
@@ -4531,13 +4564,13 @@
       <c r="K87" s="1"/>
       <c r="L87" s="10"/>
       <c r="M87" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N87" s="3"/>
       <c r="O87" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P87" s="3"/>
       <c r="Q87" s="1"/>
@@ -4556,13 +4589,13 @@
       <c r="K88" s="1"/>
       <c r="L88" s="10"/>
       <c r="M88" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N88" s="3"/>
       <c r="O88" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P88" s="3"/>
       <c r="Q88" s="1"/>
@@ -4581,13 +4614,13 @@
       <c r="K89" s="1"/>
       <c r="L89" s="10"/>
       <c r="M89" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N89" s="3"/>
       <c r="O89" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P89" s="3"/>
       <c r="Q89" s="1"/>
@@ -4606,13 +4639,13 @@
       <c r="K90" s="1"/>
       <c r="L90" s="10"/>
       <c r="M90" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N90" s="3"/>
       <c r="O90" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P90" s="3"/>
       <c r="Q90" s="1"/>
@@ -4631,13 +4664,13 @@
       <c r="K91" s="1"/>
       <c r="L91" s="10"/>
       <c r="M91" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N91" s="3"/>
       <c r="O91" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P91" s="3"/>
       <c r="Q91" s="1"/>
@@ -4656,13 +4689,13 @@
       <c r="K92" s="1"/>
       <c r="L92" s="10"/>
       <c r="M92" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N92" s="3"/>
       <c r="O92" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P92" s="3"/>
       <c r="Q92" s="1"/>
@@ -4681,13 +4714,13 @@
       <c r="K93" s="1"/>
       <c r="L93" s="10"/>
       <c r="M93" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N93" s="3"/>
       <c r="O93" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P93" s="3"/>
       <c r="Q93" s="1"/>
@@ -4706,13 +4739,13 @@
       <c r="K94" s="1"/>
       <c r="L94" s="10"/>
       <c r="M94" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N94" s="3"/>
       <c r="O94" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P94" s="3"/>
       <c r="Q94" s="1"/>
@@ -4731,13 +4764,13 @@
       <c r="K95" s="1"/>
       <c r="L95" s="10"/>
       <c r="M95" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N95" s="3"/>
       <c r="O95" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P95" s="3"/>
       <c r="Q95" s="1"/>
@@ -4756,13 +4789,13 @@
       <c r="K96" s="1"/>
       <c r="L96" s="10"/>
       <c r="M96" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N96" s="3"/>
       <c r="O96" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P96" s="3"/>
       <c r="Q96" s="1"/>
@@ -4781,13 +4814,13 @@
       <c r="K97" s="1"/>
       <c r="L97" s="10"/>
       <c r="M97" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N97" s="3"/>
       <c r="O97" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P97" s="3"/>
       <c r="Q97" s="1"/>
@@ -4806,13 +4839,13 @@
       <c r="K98" s="1"/>
       <c r="L98" s="10"/>
       <c r="M98" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N98" s="3"/>
       <c r="O98" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P98" s="3"/>
       <c r="Q98" s="1"/>
@@ -4831,13 +4864,13 @@
       <c r="K99" s="1"/>
       <c r="L99" s="10"/>
       <c r="M99" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N99" s="3"/>
       <c r="O99" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P99" s="3"/>
       <c r="Q99" s="1"/>
@@ -4856,13 +4889,13 @@
       <c r="K100" s="1"/>
       <c r="L100" s="10"/>
       <c r="M100" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N100" s="3"/>
       <c r="O100" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P100" s="3"/>
       <c r="Q100" s="1"/>
@@ -4881,13 +4914,13 @@
       <c r="K101" s="1"/>
       <c r="L101" s="10"/>
       <c r="M101" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N101" s="3"/>
       <c r="O101" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P101" s="3"/>
       <c r="Q101" s="1"/>
@@ -4906,13 +4939,13 @@
       <c r="K102" s="1"/>
       <c r="L102" s="10"/>
       <c r="M102" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N102" s="3"/>
       <c r="O102" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P102" s="3"/>
       <c r="Q102" s="1"/>
@@ -4931,13 +4964,13 @@
       <c r="K103" s="1"/>
       <c r="L103" s="10"/>
       <c r="M103" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N103" s="3"/>
       <c r="O103" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P103" s="3"/>
       <c r="Q103" s="1"/>
@@ -4956,13 +4989,13 @@
       <c r="K104" s="1"/>
       <c r="L104" s="10"/>
       <c r="M104" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N104" s="3"/>
       <c r="O104" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P104" s="3"/>
       <c r="Q104" s="1"/>
@@ -4981,13 +5014,13 @@
       <c r="K105" s="1"/>
       <c r="L105" s="10"/>
       <c r="M105" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N105" s="3"/>
       <c r="O105" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P105" s="3"/>
       <c r="Q105" s="1"/>
@@ -5006,13 +5039,13 @@
       <c r="K106" s="1"/>
       <c r="L106" s="10"/>
       <c r="M106" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N106" s="3"/>
       <c r="O106" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P106" s="3"/>
       <c r="Q106" s="1"/>
@@ -5031,13 +5064,13 @@
       <c r="K107" s="1"/>
       <c r="L107" s="10"/>
       <c r="M107" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N107" s="3"/>
       <c r="O107" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P107" s="3"/>
       <c r="Q107" s="1"/>
@@ -5056,13 +5089,13 @@
       <c r="K108" s="1"/>
       <c r="L108" s="10"/>
       <c r="M108" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N108" s="3"/>
       <c r="O108" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P108" s="3"/>
       <c r="Q108" s="1"/>
@@ -5081,13 +5114,13 @@
       <c r="K109" s="1"/>
       <c r="L109" s="10"/>
       <c r="M109" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N109" s="3"/>
       <c r="O109" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P109" s="3"/>
       <c r="Q109" s="1"/>
@@ -5106,13 +5139,13 @@
       <c r="K110" s="1"/>
       <c r="L110" s="10"/>
       <c r="M110" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N110" s="3"/>
       <c r="O110" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P110" s="3"/>
       <c r="Q110" s="1"/>
@@ -5131,13 +5164,13 @@
       <c r="K111" s="1"/>
       <c r="L111" s="10"/>
       <c r="M111" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N111" s="3"/>
       <c r="O111" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P111" s="3"/>
       <c r="Q111" s="1"/>
@@ -5156,13 +5189,13 @@
       <c r="K112" s="1"/>
       <c r="L112" s="10"/>
       <c r="M112" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N112" s="3"/>
       <c r="O112" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P112" s="3"/>
       <c r="Q112" s="1"/>
@@ -5181,13 +5214,13 @@
       <c r="K113" s="1"/>
       <c r="L113" s="10"/>
       <c r="M113" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N113" s="3"/>
       <c r="O113" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P113" s="3"/>
       <c r="Q113" s="1"/>
@@ -5206,13 +5239,13 @@
       <c r="K114" s="1"/>
       <c r="L114" s="10"/>
       <c r="M114" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N114" s="3"/>
       <c r="O114" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P114" s="3"/>
       <c r="Q114" s="1"/>
@@ -5231,13 +5264,13 @@
       <c r="K115" s="1"/>
       <c r="L115" s="10"/>
       <c r="M115" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N115" s="3"/>
       <c r="O115" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P115" s="3"/>
       <c r="Q115" s="1"/>
@@ -5256,13 +5289,13 @@
       <c r="K116" s="1"/>
       <c r="L116" s="10"/>
       <c r="M116" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N116" s="3"/>
       <c r="O116" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P116" s="3"/>
       <c r="Q116" s="1"/>
@@ -5281,13 +5314,13 @@
       <c r="K117" s="1"/>
       <c r="L117" s="10"/>
       <c r="M117" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N117" s="3"/>
       <c r="O117" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P117" s="3"/>
       <c r="Q117" s="1"/>
@@ -5306,13 +5339,13 @@
       <c r="K118" s="1"/>
       <c r="L118" s="10"/>
       <c r="M118" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N118" s="3"/>
       <c r="O118" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P118" s="3"/>
       <c r="Q118" s="1"/>
@@ -5331,13 +5364,13 @@
       <c r="K119" s="1"/>
       <c r="L119" s="10"/>
       <c r="M119" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N119" s="3"/>
       <c r="O119" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P119" s="3"/>
       <c r="Q119" s="1"/>
@@ -5356,13 +5389,13 @@
       <c r="K120" s="1"/>
       <c r="L120" s="10"/>
       <c r="M120" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N120" s="3"/>
       <c r="O120" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P120" s="3"/>
       <c r="Q120" s="1"/>
@@ -5381,13 +5414,13 @@
       <c r="K121" s="1"/>
       <c r="L121" s="10"/>
       <c r="M121" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N121" s="3"/>
       <c r="O121" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P121" s="3"/>
       <c r="Q121" s="1"/>
@@ -5406,13 +5439,13 @@
       <c r="K122" s="1"/>
       <c r="L122" s="10"/>
       <c r="M122" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N122" s="3"/>
       <c r="O122" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P122" s="3"/>
       <c r="Q122" s="1"/>
@@ -5431,13 +5464,13 @@
       <c r="K123" s="1"/>
       <c r="L123" s="10"/>
       <c r="M123" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N123" s="3"/>
       <c r="O123" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P123" s="3"/>
       <c r="Q123" s="1"/>
@@ -5456,13 +5489,13 @@
       <c r="K124" s="1"/>
       <c r="L124" s="10"/>
       <c r="M124" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N124" s="3"/>
       <c r="O124" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P124" s="3"/>
       <c r="Q124" s="1"/>
@@ -5481,13 +5514,13 @@
       <c r="K125" s="1"/>
       <c r="L125" s="10"/>
       <c r="M125" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N125" s="3"/>
       <c r="O125" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P125" s="3"/>
       <c r="Q125" s="1"/>
@@ -5506,13 +5539,13 @@
       <c r="K126" s="1"/>
       <c r="L126" s="10"/>
       <c r="M126" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N126" s="3"/>
       <c r="O126" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P126" s="3"/>
       <c r="Q126" s="1"/>
@@ -5531,13 +5564,13 @@
       <c r="K127" s="1"/>
       <c r="L127" s="10"/>
       <c r="M127" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N127" s="3"/>
       <c r="O127" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P127" s="3"/>
       <c r="Q127" s="1"/>
@@ -5556,13 +5589,13 @@
       <c r="K128" s="1"/>
       <c r="L128" s="10"/>
       <c r="M128" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N128" s="3"/>
       <c r="O128" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P128" s="3"/>
       <c r="Q128" s="1"/>
@@ -5581,13 +5614,13 @@
       <c r="K129" s="1"/>
       <c r="L129" s="10"/>
       <c r="M129" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N129" s="3"/>
       <c r="O129" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P129" s="3"/>
       <c r="Q129" s="1"/>
@@ -5606,13 +5639,13 @@
       <c r="K130" s="1"/>
       <c r="L130" s="10"/>
       <c r="M130" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N130" s="3"/>
       <c r="O130" s="3">
-        <f t="shared" si="9"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="10"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P130" s="3"/>
       <c r="Q130" s="1"/>
@@ -5631,13 +5664,13 @@
       <c r="K131" s="1"/>
       <c r="L131" s="10"/>
       <c r="M131" s="10">
-        <f t="shared" si="8"/>
-        <v>107.3</v>
+        <f t="shared" si="9"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N131" s="3"/>
       <c r="O131" s="3">
-        <f t="shared" ref="O131:O194" si="10">(M131-24.08)/24.08</f>
-        <v>3.455980066445183</v>
+        <f t="shared" ref="O131:O194" si="12">(M131-24.08)/24.08</f>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P131" s="3"/>
       <c r="Q131" s="1"/>
@@ -5656,13 +5689,13 @@
       <c r="K132" s="1"/>
       <c r="L132" s="10"/>
       <c r="M132" s="10">
-        <f t="shared" ref="M132:M195" si="11">M131+L132</f>
-        <v>107.3</v>
+        <f t="shared" ref="M132:M195" si="13">M131+L132</f>
+        <v>95.969999999999985</v>
       </c>
       <c r="N132" s="3"/>
       <c r="O132" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P132" s="3"/>
       <c r="Q132" s="1"/>
@@ -5681,13 +5714,13 @@
       <c r="K133" s="1"/>
       <c r="L133" s="10"/>
       <c r="M133" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N133" s="3"/>
       <c r="O133" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P133" s="3"/>
       <c r="Q133" s="1"/>
@@ -5706,13 +5739,13 @@
       <c r="K134" s="1"/>
       <c r="L134" s="10"/>
       <c r="M134" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N134" s="3"/>
       <c r="O134" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P134" s="3"/>
       <c r="Q134" s="1"/>
@@ -5731,13 +5764,13 @@
       <c r="K135" s="1"/>
       <c r="L135" s="10"/>
       <c r="M135" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N135" s="3"/>
       <c r="O135" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P135" s="3"/>
       <c r="Q135" s="1"/>
@@ -5756,13 +5789,13 @@
       <c r="K136" s="1"/>
       <c r="L136" s="10"/>
       <c r="M136" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N136" s="3"/>
       <c r="O136" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P136" s="3"/>
       <c r="Q136" s="1"/>
@@ -5781,13 +5814,13 @@
       <c r="K137" s="1"/>
       <c r="L137" s="10"/>
       <c r="M137" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N137" s="3"/>
       <c r="O137" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P137" s="3"/>
       <c r="Q137" s="1"/>
@@ -5806,13 +5839,13 @@
       <c r="K138" s="1"/>
       <c r="L138" s="10"/>
       <c r="M138" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N138" s="3"/>
       <c r="O138" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P138" s="3"/>
       <c r="Q138" s="1"/>
@@ -5831,13 +5864,13 @@
       <c r="K139" s="1"/>
       <c r="L139" s="10"/>
       <c r="M139" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N139" s="3"/>
       <c r="O139" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P139" s="3"/>
       <c r="Q139" s="1"/>
@@ -5856,13 +5889,13 @@
       <c r="K140" s="1"/>
       <c r="L140" s="10"/>
       <c r="M140" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N140" s="3"/>
       <c r="O140" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P140" s="3"/>
       <c r="Q140" s="1"/>
@@ -5881,13 +5914,13 @@
       <c r="K141" s="1"/>
       <c r="L141" s="10"/>
       <c r="M141" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N141" s="3"/>
       <c r="O141" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P141" s="3"/>
       <c r="Q141" s="1"/>
@@ -5906,13 +5939,13 @@
       <c r="K142" s="1"/>
       <c r="L142" s="10"/>
       <c r="M142" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N142" s="3"/>
       <c r="O142" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P142" s="3"/>
       <c r="Q142" s="1"/>
@@ -5931,13 +5964,13 @@
       <c r="K143" s="1"/>
       <c r="L143" s="10"/>
       <c r="M143" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N143" s="3"/>
       <c r="O143" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P143" s="3"/>
       <c r="Q143" s="1"/>
@@ -5956,13 +5989,13 @@
       <c r="K144" s="1"/>
       <c r="L144" s="10"/>
       <c r="M144" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N144" s="3"/>
       <c r="O144" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P144" s="3"/>
       <c r="Q144" s="1"/>
@@ -5981,13 +6014,13 @@
       <c r="K145" s="1"/>
       <c r="L145" s="10"/>
       <c r="M145" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N145" s="3"/>
       <c r="O145" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P145" s="3"/>
       <c r="Q145" s="1"/>
@@ -6006,13 +6039,13 @@
       <c r="K146" s="1"/>
       <c r="L146" s="10"/>
       <c r="M146" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N146" s="3"/>
       <c r="O146" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P146" s="3"/>
       <c r="Q146" s="1"/>
@@ -6031,13 +6064,13 @@
       <c r="K147" s="1"/>
       <c r="L147" s="10"/>
       <c r="M147" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N147" s="3"/>
       <c r="O147" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P147" s="3"/>
       <c r="Q147" s="1"/>
@@ -6056,13 +6089,13 @@
       <c r="K148" s="1"/>
       <c r="L148" s="10"/>
       <c r="M148" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N148" s="3"/>
       <c r="O148" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P148" s="3"/>
       <c r="Q148" s="1"/>
@@ -6081,13 +6114,13 @@
       <c r="K149" s="1"/>
       <c r="L149" s="10"/>
       <c r="M149" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N149" s="3"/>
       <c r="O149" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P149" s="3"/>
       <c r="Q149" s="1"/>
@@ -6106,13 +6139,13 @@
       <c r="K150" s="1"/>
       <c r="L150" s="10"/>
       <c r="M150" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N150" s="3"/>
       <c r="O150" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P150" s="3"/>
       <c r="Q150" s="1"/>
@@ -6131,13 +6164,13 @@
       <c r="K151" s="1"/>
       <c r="L151" s="10"/>
       <c r="M151" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N151" s="3"/>
       <c r="O151" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P151" s="3"/>
       <c r="Q151" s="1"/>
@@ -6156,13 +6189,13 @@
       <c r="K152" s="1"/>
       <c r="L152" s="10"/>
       <c r="M152" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N152" s="3"/>
       <c r="O152" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P152" s="3"/>
       <c r="Q152" s="1"/>
@@ -6181,13 +6214,13 @@
       <c r="K153" s="1"/>
       <c r="L153" s="10"/>
       <c r="M153" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N153" s="3"/>
       <c r="O153" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P153" s="3"/>
       <c r="Q153" s="1"/>
@@ -6206,13 +6239,13 @@
       <c r="K154" s="1"/>
       <c r="L154" s="10"/>
       <c r="M154" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N154" s="3"/>
       <c r="O154" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P154" s="3"/>
       <c r="Q154" s="1"/>
@@ -6231,13 +6264,13 @@
       <c r="K155" s="1"/>
       <c r="L155" s="10"/>
       <c r="M155" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N155" s="3"/>
       <c r="O155" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P155" s="3"/>
       <c r="Q155" s="1"/>
@@ -6256,13 +6289,13 @@
       <c r="K156" s="1"/>
       <c r="L156" s="10"/>
       <c r="M156" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N156" s="3"/>
       <c r="O156" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P156" s="3"/>
       <c r="Q156" s="1"/>
@@ -6281,13 +6314,13 @@
       <c r="K157" s="1"/>
       <c r="L157" s="10"/>
       <c r="M157" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N157" s="3"/>
       <c r="O157" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P157" s="3"/>
       <c r="Q157" s="1"/>
@@ -6306,13 +6339,13 @@
       <c r="K158" s="1"/>
       <c r="L158" s="10"/>
       <c r="M158" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N158" s="3"/>
       <c r="O158" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P158" s="3"/>
       <c r="Q158" s="1"/>
@@ -6331,13 +6364,13 @@
       <c r="K159" s="1"/>
       <c r="L159" s="10"/>
       <c r="M159" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N159" s="3"/>
       <c r="O159" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P159" s="3"/>
       <c r="Q159" s="1"/>
@@ -6356,13 +6389,13 @@
       <c r="K160" s="1"/>
       <c r="L160" s="10"/>
       <c r="M160" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N160" s="3"/>
       <c r="O160" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P160" s="3"/>
       <c r="Q160" s="1"/>
@@ -6381,13 +6414,13 @@
       <c r="K161" s="1"/>
       <c r="L161" s="10"/>
       <c r="M161" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N161" s="3"/>
       <c r="O161" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P161" s="3"/>
       <c r="Q161" s="1"/>
@@ -6406,13 +6439,13 @@
       <c r="K162" s="1"/>
       <c r="L162" s="10"/>
       <c r="M162" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N162" s="3"/>
       <c r="O162" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P162" s="3"/>
       <c r="Q162" s="1"/>
@@ -6431,13 +6464,13 @@
       <c r="K163" s="1"/>
       <c r="L163" s="10"/>
       <c r="M163" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N163" s="3"/>
       <c r="O163" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P163" s="3"/>
       <c r="Q163" s="1"/>
@@ -6456,13 +6489,13 @@
       <c r="K164" s="1"/>
       <c r="L164" s="10"/>
       <c r="M164" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N164" s="3"/>
       <c r="O164" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P164" s="3"/>
       <c r="Q164" s="1"/>
@@ -6481,13 +6514,13 @@
       <c r="K165" s="1"/>
       <c r="L165" s="10"/>
       <c r="M165" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N165" s="3"/>
       <c r="O165" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P165" s="3"/>
       <c r="Q165" s="1"/>
@@ -6506,13 +6539,13 @@
       <c r="K166" s="1"/>
       <c r="L166" s="10"/>
       <c r="M166" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N166" s="3"/>
       <c r="O166" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P166" s="3"/>
       <c r="Q166" s="1"/>
@@ -6531,13 +6564,13 @@
       <c r="K167" s="1"/>
       <c r="L167" s="10"/>
       <c r="M167" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N167" s="3"/>
       <c r="O167" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P167" s="3"/>
       <c r="Q167" s="1"/>
@@ -6556,13 +6589,13 @@
       <c r="K168" s="1"/>
       <c r="L168" s="10"/>
       <c r="M168" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N168" s="3"/>
       <c r="O168" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P168" s="3"/>
       <c r="Q168" s="1"/>
@@ -6581,13 +6614,13 @@
       <c r="K169" s="1"/>
       <c r="L169" s="10"/>
       <c r="M169" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N169" s="3"/>
       <c r="O169" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P169" s="3"/>
       <c r="Q169" s="1"/>
@@ -6606,13 +6639,13 @@
       <c r="K170" s="1"/>
       <c r="L170" s="10"/>
       <c r="M170" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N170" s="3"/>
       <c r="O170" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P170" s="3"/>
       <c r="Q170" s="1"/>
@@ -6631,13 +6664,13 @@
       <c r="K171" s="1"/>
       <c r="L171" s="10"/>
       <c r="M171" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N171" s="3"/>
       <c r="O171" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P171" s="3"/>
       <c r="Q171" s="1"/>
@@ -6656,13 +6689,13 @@
       <c r="K172" s="1"/>
       <c r="L172" s="10"/>
       <c r="M172" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N172" s="3"/>
       <c r="O172" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P172" s="3"/>
       <c r="Q172" s="1"/>
@@ -6681,13 +6714,13 @@
       <c r="K173" s="1"/>
       <c r="L173" s="10"/>
       <c r="M173" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N173" s="3"/>
       <c r="O173" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P173" s="3"/>
       <c r="Q173" s="1"/>
@@ -6706,13 +6739,13 @@
       <c r="K174" s="1"/>
       <c r="L174" s="10"/>
       <c r="M174" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N174" s="3"/>
       <c r="O174" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P174" s="3"/>
       <c r="Q174" s="1"/>
@@ -6731,13 +6764,13 @@
       <c r="K175" s="1"/>
       <c r="L175" s="10"/>
       <c r="M175" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N175" s="3"/>
       <c r="O175" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P175" s="3"/>
       <c r="Q175" s="1"/>
@@ -6756,13 +6789,13 @@
       <c r="K176" s="1"/>
       <c r="L176" s="10"/>
       <c r="M176" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N176" s="3"/>
       <c r="O176" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P176" s="3"/>
       <c r="Q176" s="1"/>
@@ -6781,13 +6814,13 @@
       <c r="K177" s="1"/>
       <c r="L177" s="10"/>
       <c r="M177" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N177" s="3"/>
       <c r="O177" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P177" s="3"/>
       <c r="Q177" s="1"/>
@@ -6806,13 +6839,13 @@
       <c r="K178" s="1"/>
       <c r="L178" s="10"/>
       <c r="M178" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N178" s="3"/>
       <c r="O178" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P178" s="3"/>
       <c r="Q178" s="1"/>
@@ -6831,13 +6864,13 @@
       <c r="K179" s="1"/>
       <c r="L179" s="10"/>
       <c r="M179" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N179" s="3"/>
       <c r="O179" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P179" s="3"/>
       <c r="Q179" s="1"/>
@@ -6856,13 +6889,13 @@
       <c r="K180" s="1"/>
       <c r="L180" s="10"/>
       <c r="M180" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N180" s="3"/>
       <c r="O180" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P180" s="3"/>
       <c r="Q180" s="1"/>
@@ -6881,13 +6914,13 @@
       <c r="K181" s="1"/>
       <c r="L181" s="10"/>
       <c r="M181" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N181" s="3"/>
       <c r="O181" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P181" s="3"/>
       <c r="Q181" s="1"/>
@@ -6906,13 +6939,13 @@
       <c r="K182" s="1"/>
       <c r="L182" s="10"/>
       <c r="M182" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N182" s="3"/>
       <c r="O182" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P182" s="3"/>
       <c r="Q182" s="1"/>
@@ -6931,13 +6964,13 @@
       <c r="K183" s="1"/>
       <c r="L183" s="10"/>
       <c r="M183" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N183" s="3"/>
       <c r="O183" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P183" s="3"/>
       <c r="Q183" s="1"/>
@@ -6956,13 +6989,13 @@
       <c r="K184" s="1"/>
       <c r="L184" s="10"/>
       <c r="M184" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N184" s="3"/>
       <c r="O184" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P184" s="3"/>
       <c r="Q184" s="1"/>
@@ -6981,13 +7014,13 @@
       <c r="K185" s="1"/>
       <c r="L185" s="10"/>
       <c r="M185" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N185" s="3"/>
       <c r="O185" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P185" s="3"/>
       <c r="Q185" s="1"/>
@@ -7006,13 +7039,13 @@
       <c r="K186" s="1"/>
       <c r="L186" s="10"/>
       <c r="M186" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N186" s="3"/>
       <c r="O186" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P186" s="3"/>
       <c r="Q186" s="1"/>
@@ -7031,13 +7064,13 @@
       <c r="K187" s="1"/>
       <c r="L187" s="10"/>
       <c r="M187" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N187" s="3"/>
       <c r="O187" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P187" s="3"/>
       <c r="Q187" s="1"/>
@@ -7056,13 +7089,13 @@
       <c r="K188" s="1"/>
       <c r="L188" s="10"/>
       <c r="M188" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N188" s="3"/>
       <c r="O188" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P188" s="3"/>
       <c r="Q188" s="1"/>
@@ -7081,13 +7114,13 @@
       <c r="K189" s="1"/>
       <c r="L189" s="10"/>
       <c r="M189" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N189" s="3"/>
       <c r="O189" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P189" s="3"/>
       <c r="Q189" s="1"/>
@@ -7106,13 +7139,13 @@
       <c r="K190" s="1"/>
       <c r="L190" s="10"/>
       <c r="M190" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N190" s="3"/>
       <c r="O190" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P190" s="3"/>
       <c r="Q190" s="1"/>
@@ -7131,13 +7164,13 @@
       <c r="K191" s="1"/>
       <c r="L191" s="10"/>
       <c r="M191" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N191" s="3"/>
       <c r="O191" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P191" s="3"/>
       <c r="Q191" s="1"/>
@@ -7156,13 +7189,13 @@
       <c r="K192" s="1"/>
       <c r="L192" s="10"/>
       <c r="M192" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N192" s="3"/>
       <c r="O192" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P192" s="3"/>
       <c r="Q192" s="1"/>
@@ -7181,13 +7214,13 @@
       <c r="K193" s="1"/>
       <c r="L193" s="10"/>
       <c r="M193" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N193" s="3"/>
       <c r="O193" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P193" s="3"/>
       <c r="Q193" s="1"/>
@@ -7206,13 +7239,13 @@
       <c r="K194" s="1"/>
       <c r="L194" s="10"/>
       <c r="M194" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N194" s="3"/>
       <c r="O194" s="3">
-        <f t="shared" si="10"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="12"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P194" s="3"/>
       <c r="Q194" s="1"/>
@@ -7231,13 +7264,13 @@
       <c r="K195" s="1"/>
       <c r="L195" s="10"/>
       <c r="M195" s="10">
-        <f t="shared" si="11"/>
-        <v>107.3</v>
+        <f t="shared" si="13"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N195" s="3"/>
       <c r="O195" s="3">
-        <f t="shared" ref="O195:O258" si="12">(M195-24.08)/24.08</f>
-        <v>3.455980066445183</v>
+        <f t="shared" ref="O195:O258" si="14">(M195-24.08)/24.08</f>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P195" s="3"/>
       <c r="Q195" s="1"/>
@@ -7256,13 +7289,13 @@
       <c r="K196" s="1"/>
       <c r="L196" s="10"/>
       <c r="M196" s="10">
-        <f t="shared" ref="M196:M259" si="13">M195+L196</f>
-        <v>107.3</v>
+        <f t="shared" ref="M196:M259" si="15">M195+L196</f>
+        <v>95.969999999999985</v>
       </c>
       <c r="N196" s="3"/>
       <c r="O196" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P196" s="3"/>
       <c r="Q196" s="1"/>
@@ -7281,13 +7314,13 @@
       <c r="K197" s="1"/>
       <c r="L197" s="10"/>
       <c r="M197" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N197" s="3"/>
       <c r="O197" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P197" s="3"/>
       <c r="Q197" s="1"/>
@@ -7306,13 +7339,13 @@
       <c r="K198" s="1"/>
       <c r="L198" s="10"/>
       <c r="M198" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N198" s="3"/>
       <c r="O198" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P198" s="3"/>
       <c r="Q198" s="1"/>
@@ -7331,13 +7364,13 @@
       <c r="K199" s="1"/>
       <c r="L199" s="10"/>
       <c r="M199" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N199" s="3"/>
       <c r="O199" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P199" s="3"/>
       <c r="Q199" s="1"/>
@@ -7356,13 +7389,13 @@
       <c r="K200" s="1"/>
       <c r="L200" s="10"/>
       <c r="M200" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N200" s="3"/>
       <c r="O200" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P200" s="3"/>
       <c r="Q200" s="1"/>
@@ -7381,13 +7414,13 @@
       <c r="K201" s="1"/>
       <c r="L201" s="10"/>
       <c r="M201" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N201" s="3"/>
       <c r="O201" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P201" s="3"/>
       <c r="Q201" s="1"/>
@@ -7406,13 +7439,13 @@
       <c r="K202" s="1"/>
       <c r="L202" s="10"/>
       <c r="M202" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N202" s="3"/>
       <c r="O202" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P202" s="3"/>
       <c r="Q202" s="1"/>
@@ -7431,13 +7464,13 @@
       <c r="K203" s="1"/>
       <c r="L203" s="10"/>
       <c r="M203" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N203" s="3"/>
       <c r="O203" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P203" s="3"/>
       <c r="Q203" s="1"/>
@@ -7456,13 +7489,13 @@
       <c r="K204" s="1"/>
       <c r="L204" s="10"/>
       <c r="M204" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N204" s="3"/>
       <c r="O204" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P204" s="3"/>
       <c r="Q204" s="1"/>
@@ -7481,13 +7514,13 @@
       <c r="K205" s="1"/>
       <c r="L205" s="10"/>
       <c r="M205" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N205" s="3"/>
       <c r="O205" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P205" s="3"/>
       <c r="Q205" s="1"/>
@@ -7506,13 +7539,13 @@
       <c r="K206" s="1"/>
       <c r="L206" s="10"/>
       <c r="M206" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N206" s="3"/>
       <c r="O206" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P206" s="3"/>
       <c r="Q206" s="1"/>
@@ -7531,13 +7564,13 @@
       <c r="K207" s="1"/>
       <c r="L207" s="10"/>
       <c r="M207" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N207" s="3"/>
       <c r="O207" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P207" s="3"/>
       <c r="Q207" s="1"/>
@@ -7556,13 +7589,13 @@
       <c r="K208" s="1"/>
       <c r="L208" s="10"/>
       <c r="M208" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N208" s="3"/>
       <c r="O208" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P208" s="3"/>
       <c r="Q208" s="1"/>
@@ -7581,13 +7614,13 @@
       <c r="K209" s="1"/>
       <c r="L209" s="10"/>
       <c r="M209" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N209" s="3"/>
       <c r="O209" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P209" s="3"/>
       <c r="Q209" s="1"/>
@@ -7606,13 +7639,13 @@
       <c r="K210" s="1"/>
       <c r="L210" s="10"/>
       <c r="M210" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N210" s="3"/>
       <c r="O210" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P210" s="3"/>
       <c r="Q210" s="1"/>
@@ -7631,13 +7664,13 @@
       <c r="K211" s="1"/>
       <c r="L211" s="10"/>
       <c r="M211" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N211" s="3"/>
       <c r="O211" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P211" s="3"/>
       <c r="Q211" s="1"/>
@@ -7656,13 +7689,13 @@
       <c r="K212" s="1"/>
       <c r="L212" s="10"/>
       <c r="M212" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N212" s="3"/>
       <c r="O212" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P212" s="3"/>
       <c r="Q212" s="1"/>
@@ -7681,13 +7714,13 @@
       <c r="K213" s="1"/>
       <c r="L213" s="10"/>
       <c r="M213" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N213" s="3"/>
       <c r="O213" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P213" s="3"/>
       <c r="Q213" s="1"/>
@@ -7706,13 +7739,13 @@
       <c r="K214" s="1"/>
       <c r="L214" s="10"/>
       <c r="M214" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N214" s="3"/>
       <c r="O214" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P214" s="3"/>
       <c r="Q214" s="1"/>
@@ -7731,13 +7764,13 @@
       <c r="K215" s="1"/>
       <c r="L215" s="10"/>
       <c r="M215" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N215" s="3"/>
       <c r="O215" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P215" s="3"/>
       <c r="Q215" s="1"/>
@@ -7756,13 +7789,13 @@
       <c r="K216" s="1"/>
       <c r="L216" s="10"/>
       <c r="M216" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N216" s="3"/>
       <c r="O216" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P216" s="3"/>
       <c r="Q216" s="1"/>
@@ -7781,13 +7814,13 @@
       <c r="K217" s="1"/>
       <c r="L217" s="10"/>
       <c r="M217" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N217" s="3"/>
       <c r="O217" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P217" s="3"/>
       <c r="Q217" s="1"/>
@@ -7806,13 +7839,13 @@
       <c r="K218" s="1"/>
       <c r="L218" s="10"/>
       <c r="M218" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N218" s="3"/>
       <c r="O218" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P218" s="3"/>
       <c r="Q218" s="1"/>
@@ -7831,13 +7864,13 @@
       <c r="K219" s="1"/>
       <c r="L219" s="10"/>
       <c r="M219" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N219" s="3"/>
       <c r="O219" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P219" s="3"/>
       <c r="Q219" s="1"/>
@@ -7856,13 +7889,13 @@
       <c r="K220" s="1"/>
       <c r="L220" s="10"/>
       <c r="M220" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N220" s="3"/>
       <c r="O220" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P220" s="3"/>
       <c r="Q220" s="1"/>
@@ -7881,13 +7914,13 @@
       <c r="K221" s="1"/>
       <c r="L221" s="10"/>
       <c r="M221" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N221" s="3"/>
       <c r="O221" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P221" s="3"/>
       <c r="Q221" s="1"/>
@@ -7906,13 +7939,13 @@
       <c r="K222" s="1"/>
       <c r="L222" s="10"/>
       <c r="M222" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N222" s="3"/>
       <c r="O222" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P222" s="3"/>
       <c r="Q222" s="1"/>
@@ -7931,13 +7964,13 @@
       <c r="K223" s="1"/>
       <c r="L223" s="10"/>
       <c r="M223" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N223" s="3"/>
       <c r="O223" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P223" s="3"/>
       <c r="Q223" s="1"/>
@@ -7956,13 +7989,13 @@
       <c r="K224" s="1"/>
       <c r="L224" s="10"/>
       <c r="M224" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N224" s="3"/>
       <c r="O224" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P224" s="3"/>
       <c r="Q224" s="1"/>
@@ -7981,13 +8014,13 @@
       <c r="K225" s="1"/>
       <c r="L225" s="10"/>
       <c r="M225" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N225" s="3"/>
       <c r="O225" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P225" s="3"/>
       <c r="Q225" s="1"/>
@@ -8006,13 +8039,13 @@
       <c r="K226" s="1"/>
       <c r="L226" s="10"/>
       <c r="M226" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N226" s="3"/>
       <c r="O226" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P226" s="3"/>
       <c r="Q226" s="1"/>
@@ -8031,13 +8064,13 @@
       <c r="K227" s="1"/>
       <c r="L227" s="10"/>
       <c r="M227" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N227" s="3"/>
       <c r="O227" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P227" s="3"/>
       <c r="Q227" s="1"/>
@@ -8056,13 +8089,13 @@
       <c r="K228" s="1"/>
       <c r="L228" s="10"/>
       <c r="M228" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N228" s="3"/>
       <c r="O228" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P228" s="3"/>
       <c r="Q228" s="1"/>
@@ -8081,13 +8114,13 @@
       <c r="K229" s="1"/>
       <c r="L229" s="10"/>
       <c r="M229" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N229" s="3"/>
       <c r="O229" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P229" s="3"/>
       <c r="Q229" s="1"/>
@@ -8106,13 +8139,13 @@
       <c r="K230" s="1"/>
       <c r="L230" s="10"/>
       <c r="M230" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N230" s="3"/>
       <c r="O230" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P230" s="3"/>
       <c r="Q230" s="1"/>
@@ -8131,13 +8164,13 @@
       <c r="K231" s="1"/>
       <c r="L231" s="10"/>
       <c r="M231" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N231" s="3"/>
       <c r="O231" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P231" s="3"/>
       <c r="Q231" s="1"/>
@@ -8156,13 +8189,13 @@
       <c r="K232" s="1"/>
       <c r="L232" s="10"/>
       <c r="M232" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N232" s="3"/>
       <c r="O232" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P232" s="3"/>
       <c r="Q232" s="1"/>
@@ -8181,13 +8214,13 @@
       <c r="K233" s="1"/>
       <c r="L233" s="10"/>
       <c r="M233" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N233" s="3"/>
       <c r="O233" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P233" s="3"/>
       <c r="Q233" s="1"/>
@@ -8206,13 +8239,13 @@
       <c r="K234" s="1"/>
       <c r="L234" s="10"/>
       <c r="M234" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N234" s="3"/>
       <c r="O234" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P234" s="3"/>
       <c r="Q234" s="1"/>
@@ -8231,13 +8264,13 @@
       <c r="K235" s="1"/>
       <c r="L235" s="10"/>
       <c r="M235" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N235" s="3"/>
       <c r="O235" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P235" s="3"/>
       <c r="Q235" s="1"/>
@@ -8256,13 +8289,13 @@
       <c r="K236" s="1"/>
       <c r="L236" s="10"/>
       <c r="M236" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N236" s="3"/>
       <c r="O236" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P236" s="3"/>
       <c r="Q236" s="1"/>
@@ -8281,13 +8314,13 @@
       <c r="K237" s="1"/>
       <c r="L237" s="10"/>
       <c r="M237" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N237" s="3"/>
       <c r="O237" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P237" s="3"/>
       <c r="Q237" s="1"/>
@@ -8306,13 +8339,13 @@
       <c r="K238" s="1"/>
       <c r="L238" s="10"/>
       <c r="M238" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N238" s="3"/>
       <c r="O238" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P238" s="3"/>
       <c r="Q238" s="1"/>
@@ -8331,13 +8364,13 @@
       <c r="K239" s="1"/>
       <c r="L239" s="10"/>
       <c r="M239" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N239" s="3"/>
       <c r="O239" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P239" s="3"/>
       <c r="Q239" s="1"/>
@@ -8356,13 +8389,13 @@
       <c r="K240" s="1"/>
       <c r="L240" s="10"/>
       <c r="M240" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N240" s="3"/>
       <c r="O240" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P240" s="3"/>
       <c r="Q240" s="1"/>
@@ -8381,13 +8414,13 @@
       <c r="K241" s="1"/>
       <c r="L241" s="10"/>
       <c r="M241" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N241" s="3"/>
       <c r="O241" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P241" s="3"/>
       <c r="Q241" s="1"/>
@@ -8406,13 +8439,13 @@
       <c r="K242" s="1"/>
       <c r="L242" s="10"/>
       <c r="M242" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N242" s="3"/>
       <c r="O242" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P242" s="3"/>
       <c r="Q242" s="1"/>
@@ -8431,13 +8464,13 @@
       <c r="K243" s="1"/>
       <c r="L243" s="10"/>
       <c r="M243" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N243" s="3"/>
       <c r="O243" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P243" s="3"/>
       <c r="Q243" s="1"/>
@@ -8456,13 +8489,13 @@
       <c r="K244" s="1"/>
       <c r="L244" s="10"/>
       <c r="M244" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N244" s="3"/>
       <c r="O244" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P244" s="3"/>
       <c r="Q244" s="1"/>
@@ -8481,13 +8514,13 @@
       <c r="K245" s="1"/>
       <c r="L245" s="10"/>
       <c r="M245" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N245" s="3"/>
       <c r="O245" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P245" s="3"/>
       <c r="Q245" s="1"/>
@@ -8506,13 +8539,13 @@
       <c r="K246" s="1"/>
       <c r="L246" s="10"/>
       <c r="M246" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N246" s="3"/>
       <c r="O246" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P246" s="3"/>
       <c r="Q246" s="1"/>
@@ -8531,13 +8564,13 @@
       <c r="K247" s="1"/>
       <c r="L247" s="10"/>
       <c r="M247" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N247" s="3"/>
       <c r="O247" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P247" s="3"/>
       <c r="Q247" s="1"/>
@@ -8556,13 +8589,13 @@
       <c r="K248" s="1"/>
       <c r="L248" s="10"/>
       <c r="M248" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N248" s="3"/>
       <c r="O248" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P248" s="3"/>
       <c r="Q248" s="1"/>
@@ -8581,13 +8614,13 @@
       <c r="K249" s="1"/>
       <c r="L249" s="10"/>
       <c r="M249" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N249" s="3"/>
       <c r="O249" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P249" s="3"/>
       <c r="Q249" s="1"/>
@@ -8606,13 +8639,13 @@
       <c r="K250" s="1"/>
       <c r="L250" s="10"/>
       <c r="M250" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N250" s="3"/>
       <c r="O250" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P250" s="3"/>
       <c r="Q250" s="1"/>
@@ -8631,13 +8664,13 @@
       <c r="K251" s="1"/>
       <c r="L251" s="10"/>
       <c r="M251" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N251" s="3"/>
       <c r="O251" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P251" s="3"/>
       <c r="Q251" s="1"/>
@@ -8656,13 +8689,13 @@
       <c r="K252" s="1"/>
       <c r="L252" s="10"/>
       <c r="M252" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N252" s="3"/>
       <c r="O252" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P252" s="3"/>
       <c r="Q252" s="1"/>
@@ -8681,13 +8714,13 @@
       <c r="K253" s="1"/>
       <c r="L253" s="10"/>
       <c r="M253" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N253" s="3"/>
       <c r="O253" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P253" s="3"/>
       <c r="Q253" s="1"/>
@@ -8706,13 +8739,13 @@
       <c r="K254" s="1"/>
       <c r="L254" s="10"/>
       <c r="M254" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N254" s="3"/>
       <c r="O254" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P254" s="3"/>
       <c r="Q254" s="1"/>
@@ -8731,13 +8764,13 @@
       <c r="K255" s="1"/>
       <c r="L255" s="10"/>
       <c r="M255" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N255" s="3"/>
       <c r="O255" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P255" s="3"/>
       <c r="Q255" s="1"/>
@@ -8756,13 +8789,13 @@
       <c r="K256" s="1"/>
       <c r="L256" s="10"/>
       <c r="M256" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N256" s="3"/>
       <c r="O256" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P256" s="3"/>
       <c r="Q256" s="1"/>
@@ -8781,13 +8814,13 @@
       <c r="K257" s="1"/>
       <c r="L257" s="10"/>
       <c r="M257" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N257" s="3"/>
       <c r="O257" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P257" s="3"/>
       <c r="Q257" s="1"/>
@@ -8806,13 +8839,13 @@
       <c r="K258" s="1"/>
       <c r="L258" s="10"/>
       <c r="M258" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N258" s="3"/>
       <c r="O258" s="3">
-        <f t="shared" si="12"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="14"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P258" s="3"/>
       <c r="Q258" s="1"/>
@@ -8831,13 +8864,13 @@
       <c r="K259" s="1"/>
       <c r="L259" s="10"/>
       <c r="M259" s="10">
-        <f t="shared" si="13"/>
-        <v>107.3</v>
+        <f t="shared" si="15"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N259" s="3"/>
       <c r="O259" s="3">
-        <f t="shared" ref="O259:O300" si="14">(M259-24.08)/24.08</f>
-        <v>3.455980066445183</v>
+        <f t="shared" ref="O259:O300" si="16">(M259-24.08)/24.08</f>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P259" s="3"/>
       <c r="Q259" s="1"/>
@@ -8856,13 +8889,13 @@
       <c r="K260" s="1"/>
       <c r="L260" s="10"/>
       <c r="M260" s="10">
-        <f t="shared" ref="M260:M300" si="15">M259+L260</f>
-        <v>107.3</v>
+        <f t="shared" ref="M260:M300" si="17">M259+L260</f>
+        <v>95.969999999999985</v>
       </c>
       <c r="N260" s="3"/>
       <c r="O260" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P260" s="3"/>
       <c r="Q260" s="1"/>
@@ -8881,13 +8914,13 @@
       <c r="K261" s="1"/>
       <c r="L261" s="10"/>
       <c r="M261" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N261" s="3"/>
       <c r="O261" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P261" s="3"/>
       <c r="Q261" s="1"/>
@@ -8906,13 +8939,13 @@
       <c r="K262" s="1"/>
       <c r="L262" s="10"/>
       <c r="M262" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N262" s="3"/>
       <c r="O262" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P262" s="3"/>
       <c r="Q262" s="1"/>
@@ -8931,13 +8964,13 @@
       <c r="K263" s="1"/>
       <c r="L263" s="10"/>
       <c r="M263" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N263" s="3"/>
       <c r="O263" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P263" s="3"/>
       <c r="Q263" s="1"/>
@@ -8956,13 +8989,13 @@
       <c r="K264" s="1"/>
       <c r="L264" s="10"/>
       <c r="M264" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N264" s="3"/>
       <c r="O264" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P264" s="3"/>
       <c r="Q264" s="1"/>
@@ -8981,13 +9014,13 @@
       <c r="K265" s="1"/>
       <c r="L265" s="10"/>
       <c r="M265" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N265" s="3"/>
       <c r="O265" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P265" s="3"/>
       <c r="Q265" s="1"/>
@@ -9006,13 +9039,13 @@
       <c r="K266" s="1"/>
       <c r="L266" s="10"/>
       <c r="M266" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N266" s="3"/>
       <c r="O266" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P266" s="3"/>
       <c r="Q266" s="1"/>
@@ -9031,13 +9064,13 @@
       <c r="K267" s="1"/>
       <c r="L267" s="10"/>
       <c r="M267" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N267" s="3"/>
       <c r="O267" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P267" s="3"/>
       <c r="Q267" s="1"/>
@@ -9056,13 +9089,13 @@
       <c r="K268" s="1"/>
       <c r="L268" s="10"/>
       <c r="M268" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N268" s="3"/>
       <c r="O268" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P268" s="3"/>
       <c r="Q268" s="1"/>
@@ -9081,13 +9114,13 @@
       <c r="K269" s="1"/>
       <c r="L269" s="10"/>
       <c r="M269" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N269" s="3"/>
       <c r="O269" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P269" s="3"/>
       <c r="Q269" s="1"/>
@@ -9106,13 +9139,13 @@
       <c r="K270" s="1"/>
       <c r="L270" s="10"/>
       <c r="M270" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N270" s="3"/>
       <c r="O270" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P270" s="3"/>
       <c r="Q270" s="1"/>
@@ -9131,13 +9164,13 @@
       <c r="K271" s="1"/>
       <c r="L271" s="10"/>
       <c r="M271" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N271" s="3"/>
       <c r="O271" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P271" s="3"/>
       <c r="Q271" s="1"/>
@@ -9156,13 +9189,13 @@
       <c r="K272" s="1"/>
       <c r="L272" s="10"/>
       <c r="M272" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N272" s="3"/>
       <c r="O272" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P272" s="3"/>
       <c r="Q272" s="1"/>
@@ -9181,13 +9214,13 @@
       <c r="K273" s="1"/>
       <c r="L273" s="10"/>
       <c r="M273" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N273" s="3"/>
       <c r="O273" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P273" s="3"/>
       <c r="Q273" s="1"/>
@@ -9206,13 +9239,13 @@
       <c r="K274" s="1"/>
       <c r="L274" s="10"/>
       <c r="M274" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N274" s="3"/>
       <c r="O274" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P274" s="3"/>
       <c r="Q274" s="1"/>
@@ -9231,13 +9264,13 @@
       <c r="K275" s="1"/>
       <c r="L275" s="10"/>
       <c r="M275" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N275" s="3"/>
       <c r="O275" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P275" s="3"/>
       <c r="Q275" s="1"/>
@@ -9256,13 +9289,13 @@
       <c r="K276" s="1"/>
       <c r="L276" s="10"/>
       <c r="M276" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N276" s="3"/>
       <c r="O276" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P276" s="3"/>
       <c r="Q276" s="1"/>
@@ -9281,13 +9314,13 @@
       <c r="K277" s="1"/>
       <c r="L277" s="10"/>
       <c r="M277" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N277" s="3"/>
       <c r="O277" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P277" s="3"/>
       <c r="Q277" s="1"/>
@@ -9306,13 +9339,13 @@
       <c r="K278" s="1"/>
       <c r="L278" s="10"/>
       <c r="M278" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N278" s="3"/>
       <c r="O278" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P278" s="3"/>
       <c r="Q278" s="1"/>
@@ -9331,13 +9364,13 @@
       <c r="K279" s="1"/>
       <c r="L279" s="10"/>
       <c r="M279" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N279" s="3"/>
       <c r="O279" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P279" s="3"/>
       <c r="Q279" s="1"/>
@@ -9356,13 +9389,13 @@
       <c r="K280" s="1"/>
       <c r="L280" s="10"/>
       <c r="M280" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N280" s="3"/>
       <c r="O280" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P280" s="3"/>
       <c r="Q280" s="1"/>
@@ -9381,13 +9414,13 @@
       <c r="K281" s="1"/>
       <c r="L281" s="10"/>
       <c r="M281" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N281" s="3"/>
       <c r="O281" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P281" s="3"/>
       <c r="Q281" s="1"/>
@@ -9406,13 +9439,13 @@
       <c r="K282" s="1"/>
       <c r="L282" s="10"/>
       <c r="M282" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N282" s="3"/>
       <c r="O282" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P282" s="3"/>
       <c r="Q282" s="1"/>
@@ -9431,13 +9464,13 @@
       <c r="K283" s="1"/>
       <c r="L283" s="10"/>
       <c r="M283" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N283" s="3"/>
       <c r="O283" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P283" s="3"/>
       <c r="Q283" s="1"/>
@@ -9456,13 +9489,13 @@
       <c r="K284" s="1"/>
       <c r="L284" s="10"/>
       <c r="M284" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N284" s="3"/>
       <c r="O284" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P284" s="3"/>
       <c r="Q284" s="1"/>
@@ -9481,13 +9514,13 @@
       <c r="K285" s="1"/>
       <c r="L285" s="10"/>
       <c r="M285" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N285" s="3"/>
       <c r="O285" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P285" s="3"/>
       <c r="Q285" s="1"/>
@@ -9506,13 +9539,13 @@
       <c r="K286" s="1"/>
       <c r="L286" s="10"/>
       <c r="M286" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N286" s="3"/>
       <c r="O286" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P286" s="3"/>
       <c r="Q286" s="1"/>
@@ -9531,13 +9564,13 @@
       <c r="K287" s="1"/>
       <c r="L287" s="10"/>
       <c r="M287" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N287" s="3"/>
       <c r="O287" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P287" s="3"/>
       <c r="Q287" s="1"/>
@@ -9556,13 +9589,13 @@
       <c r="K288" s="1"/>
       <c r="L288" s="10"/>
       <c r="M288" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N288" s="3"/>
       <c r="O288" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P288" s="3"/>
       <c r="Q288" s="1"/>
@@ -9581,13 +9614,13 @@
       <c r="K289" s="1"/>
       <c r="L289" s="10"/>
       <c r="M289" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N289" s="3"/>
       <c r="O289" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P289" s="3"/>
       <c r="Q289" s="1"/>
@@ -9606,13 +9639,13 @@
       <c r="K290" s="1"/>
       <c r="L290" s="10"/>
       <c r="M290" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N290" s="3"/>
       <c r="O290" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P290" s="3"/>
       <c r="Q290" s="1"/>
@@ -9631,13 +9664,13 @@
       <c r="K291" s="1"/>
       <c r="L291" s="10"/>
       <c r="M291" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N291" s="3"/>
       <c r="O291" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P291" s="3"/>
       <c r="Q291" s="1"/>
@@ -9656,13 +9689,13 @@
       <c r="K292" s="1"/>
       <c r="L292" s="10"/>
       <c r="M292" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N292" s="3"/>
       <c r="O292" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P292" s="3"/>
       <c r="Q292" s="1"/>
@@ -9681,13 +9714,13 @@
       <c r="K293" s="1"/>
       <c r="L293" s="10"/>
       <c r="M293" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N293" s="3"/>
       <c r="O293" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P293" s="3"/>
       <c r="Q293" s="1"/>
@@ -9706,13 +9739,13 @@
       <c r="K294" s="1"/>
       <c r="L294" s="10"/>
       <c r="M294" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N294" s="3"/>
       <c r="O294" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P294" s="3"/>
       <c r="Q294" s="1"/>
@@ -9731,13 +9764,13 @@
       <c r="K295" s="1"/>
       <c r="L295" s="10"/>
       <c r="M295" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N295" s="3"/>
       <c r="O295" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P295" s="3"/>
       <c r="Q295" s="1"/>
@@ -9756,13 +9789,13 @@
       <c r="K296" s="1"/>
       <c r="L296" s="10"/>
       <c r="M296" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N296" s="3"/>
       <c r="O296" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P296" s="3"/>
       <c r="Q296" s="1"/>
@@ -9781,13 +9814,13 @@
       <c r="K297" s="1"/>
       <c r="L297" s="10"/>
       <c r="M297" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N297" s="3"/>
       <c r="O297" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P297" s="3"/>
       <c r="Q297" s="1"/>
@@ -9806,13 +9839,13 @@
       <c r="K298" s="1"/>
       <c r="L298" s="10"/>
       <c r="M298" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N298" s="3"/>
       <c r="O298" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P298" s="3"/>
       <c r="Q298" s="1"/>
@@ -9831,13 +9864,13 @@
       <c r="K299" s="1"/>
       <c r="L299" s="10"/>
       <c r="M299" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N299" s="3"/>
       <c r="O299" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P299" s="3"/>
       <c r="Q299" s="1"/>
@@ -9856,13 +9889,13 @@
       <c r="K300" s="1"/>
       <c r="L300" s="10"/>
       <c r="M300" s="10">
-        <f t="shared" si="15"/>
-        <v>107.3</v>
+        <f t="shared" si="17"/>
+        <v>95.969999999999985</v>
       </c>
       <c r="N300" s="3"/>
       <c r="O300" s="3">
-        <f t="shared" si="14"/>
-        <v>3.455980066445183</v>
+        <f t="shared" si="16"/>
+        <v>2.9854651162790695</v>
       </c>
       <c r="P300" s="3"/>
       <c r="Q300" s="1"/>

</xml_diff>